<commit_message>
change le chemin du fichier des stations onde
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCB299E-7798-445D-B8F6-A51749879975}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327874B1-75B2-433D-B3E6-CD279E7A9BD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="7656" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -427,14 +427,14 @@
     <t>texte: Bulletin de situation hydrologique; lien:https://www.eaufrance.fr/publications/bsh</t>
   </si>
   <si>
-    <t>data-raw\stations_onde.gpkg</t>
+    <t>data-raw/stations_onde.gpkg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,13 +461,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -985,32 +978,32 @@
   <dimension ref="A1:AF23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="11.42578125" style="4"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
-    <col min="7" max="10" width="15.7109375" customWidth="1"/>
+    <col min="1" max="3" width="11.44140625" style="4"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="25.88671875" customWidth="1"/>
+    <col min="7" max="10" width="15.6640625" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="21.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1"/>
-    <col min="18" max="19" width="14.85546875" customWidth="1"/>
-    <col min="20" max="21" width="20.85546875" customWidth="1"/>
-    <col min="22" max="22" width="38.5703125" customWidth="1"/>
+    <col min="12" max="12" width="21.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" customWidth="1"/>
+    <col min="14" max="14" width="15.5546875" customWidth="1"/>
+    <col min="18" max="19" width="14.88671875" customWidth="1"/>
+    <col min="20" max="21" width="20.88671875" customWidth="1"/>
+    <col min="22" max="22" width="38.5546875" customWidth="1"/>
     <col min="24" max="24" width="16" customWidth="1"/>
-    <col min="25" max="25" width="18.140625" customWidth="1"/>
-    <col min="27" max="29" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.109375" customWidth="1"/>
+    <col min="27" max="29" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>41</v>
       </c>
@@ -1108,7 +1101,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="330" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" ht="288" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1197,7 +1190,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -1227,7 +1220,7 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1257,7 +1250,7 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -1287,7 +1280,7 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -1317,7 +1310,7 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1347,7 +1340,7 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:32" ht="210" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
@@ -1437,7 +1430,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
@@ -1467,7 +1460,7 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1497,7 +1490,7 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>19</v>
       </c>
@@ -1527,7 +1520,7 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
@@ -1557,7 +1550,7 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
@@ -1587,7 +1580,7 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
@@ -1617,7 +1610,7 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
@@ -1647,7 +1640,7 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
@@ -1677,7 +1670,7 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1707,7 +1700,7 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
@@ -1737,7 +1730,7 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>16</v>
       </c>
@@ -1767,7 +1760,7 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>17</v>
       </c>
@@ -1797,7 +1790,7 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>18</v>
       </c>
@@ -1827,7 +1820,7 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
@@ -1857,7 +1850,7 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
complète la liste des suivis
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327874B1-75B2-433D-B3E6-CD279E7A9BD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030E01C3-5E0F-434E-B0D0-3A6047B25160}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="7656" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>onde</t>
   </si>
@@ -36,9 +36,6 @@
     <t>bocage</t>
   </si>
   <si>
-    <t>carhyce</t>
-  </si>
-  <si>
     <t>castor</t>
   </si>
   <si>
@@ -51,15 +48,9 @@
     <t>chat</t>
   </si>
   <si>
-    <t>pmcc</t>
-  </si>
-  <si>
     <t>sagir</t>
   </si>
   <si>
-    <t>peches</t>
-  </si>
-  <si>
     <t>macroinvertebres</t>
   </si>
   <si>
@@ -82,9 +73,6 @@
   </si>
   <si>
     <t>thermie</t>
-  </si>
-  <si>
-    <t>geobs</t>
   </si>
   <si>
     <t>hydromorphologie</t>
@@ -428,6 +416,21 @@
   </si>
   <si>
     <t>data-raw/stations_onde.gpkg</t>
+  </si>
+  <si>
+    <t>ongules</t>
+  </si>
+  <si>
+    <t>poissons</t>
+  </si>
+  <si>
+    <t>adne</t>
+  </si>
+  <si>
+    <t>continuites</t>
+  </si>
+  <si>
+    <t>pmc</t>
   </si>
 </sst>
 </file>
@@ -638,8 +641,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B84CBB1B-C38F-41A7-A936-743876B1F305}" name="Tableau1" displayName="Tableau1" ref="A1:AF23" totalsRowShown="0">
-  <autoFilter ref="A1:AF23" xr:uid="{EF1B83D5-E66B-47E5-BA3E-4C83D3ECD89E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B84CBB1B-C38F-41A7-A936-743876B1F305}" name="Tableau1" displayName="Tableau1" ref="A1:AF24" totalsRowShown="0">
+  <autoFilter ref="A1:AF24" xr:uid="{EF1B83D5-E66B-47E5-BA3E-4C83D3ECD89E}"/>
   <tableColumns count="32">
     <tableColumn id="1" xr3:uid="{5B39F531-B957-45E4-B8D7-A8EF89A02254}" name="suivi" dataDxfId="31"/>
     <tableColumn id="25" xr3:uid="{782941AC-FB8B-4754-8CBF-02D0BAF2941E}" name="intitule" dataDxfId="30"/>
@@ -975,13 +978,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C57DFD-1CB4-4BB6-806B-B3A954B7C9AD}">
-  <dimension ref="A1:AF23"/>
+  <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1005,194 +1008,135 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="R1" t="s">
         <v>49</v>
       </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
         <v>50</v>
       </c>
-      <c r="O1" t="s">
+      <c r="T1" t="s">
         <v>51</v>
       </c>
-      <c r="P1" t="s">
+      <c r="U1" t="s">
         <v>52</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="V1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W1" t="s">
+        <v>54</v>
+      </c>
+      <c r="X1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="R1" t="s">
-        <v>53</v>
-      </c>
-      <c r="S1" t="s">
-        <v>54</v>
-      </c>
-      <c r="T1" t="s">
-        <v>55</v>
-      </c>
-      <c r="U1" t="s">
-        <v>56</v>
-      </c>
-      <c r="V1" t="s">
-        <v>57</v>
-      </c>
-      <c r="W1" t="s">
-        <v>58</v>
-      </c>
-      <c r="X1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" ht="288" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="11">
-        <v>77</v>
-      </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="W2" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="X2" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y2" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z2" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA2" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB2" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="AC2" s="11"/>
-      <c r="AD2" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="AE2" s="11" t="s">
-        <v>76</v>
-      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1222,18 +1166,18 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="1"/>
+      <c r="D4" s="2"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="2"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="K4" s="8"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -1243,12 +1187,12 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
+      <c r="U4" s="8"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
+      <c r="Z4" s="8"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
@@ -1280,39 +1224,98 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
+    <row r="6" spans="1:32" ht="288" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="11">
+        <v>77</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q6" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="S6" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="U6" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="V6" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="X6" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA6" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB6" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE6" s="11" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1340,105 +1343,45 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:32" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="O8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="U8" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y8" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z8" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA8" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB8" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AC8" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AD8" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="3"/>
+      <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1492,7 +1435,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1514,7 +1457,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
-      <c r="V11" s="6"/>
+      <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
@@ -1522,7 +1465,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1552,7 +1495,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1582,7 +1525,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1612,7 +1555,7 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1642,7 +1585,7 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1670,9 +1613,9 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1700,39 +1643,99 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U18" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z18" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD18" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="1"/>
-      <c r="X18" s="1"/>
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1760,9 +1763,9 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1784,15 +1787,15 @@
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
+      <c r="V20" s="6"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1820,9 +1823,9 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1850,9 +1853,9 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1880,6 +1883,36 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@44dd05a5feb0a4e1ba56f00a7ce504ac38203d2d 🚀
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327874B1-75B2-433D-B3E6-CD279E7A9BD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030E01C3-5E0F-434E-B0D0-3A6047B25160}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="7656" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>onde</t>
   </si>
@@ -36,9 +36,6 @@
     <t>bocage</t>
   </si>
   <si>
-    <t>carhyce</t>
-  </si>
-  <si>
     <t>castor</t>
   </si>
   <si>
@@ -51,15 +48,9 @@
     <t>chat</t>
   </si>
   <si>
-    <t>pmcc</t>
-  </si>
-  <si>
     <t>sagir</t>
   </si>
   <si>
-    <t>peches</t>
-  </si>
-  <si>
     <t>macroinvertebres</t>
   </si>
   <si>
@@ -82,9 +73,6 @@
   </si>
   <si>
     <t>thermie</t>
-  </si>
-  <si>
-    <t>geobs</t>
   </si>
   <si>
     <t>hydromorphologie</t>
@@ -428,6 +416,21 @@
   </si>
   <si>
     <t>data-raw/stations_onde.gpkg</t>
+  </si>
+  <si>
+    <t>ongules</t>
+  </si>
+  <si>
+    <t>poissons</t>
+  </si>
+  <si>
+    <t>adne</t>
+  </si>
+  <si>
+    <t>continuites</t>
+  </si>
+  <si>
+    <t>pmc</t>
   </si>
 </sst>
 </file>
@@ -638,8 +641,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B84CBB1B-C38F-41A7-A936-743876B1F305}" name="Tableau1" displayName="Tableau1" ref="A1:AF23" totalsRowShown="0">
-  <autoFilter ref="A1:AF23" xr:uid="{EF1B83D5-E66B-47E5-BA3E-4C83D3ECD89E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B84CBB1B-C38F-41A7-A936-743876B1F305}" name="Tableau1" displayName="Tableau1" ref="A1:AF24" totalsRowShown="0">
+  <autoFilter ref="A1:AF24" xr:uid="{EF1B83D5-E66B-47E5-BA3E-4C83D3ECD89E}"/>
   <tableColumns count="32">
     <tableColumn id="1" xr3:uid="{5B39F531-B957-45E4-B8D7-A8EF89A02254}" name="suivi" dataDxfId="31"/>
     <tableColumn id="25" xr3:uid="{782941AC-FB8B-4754-8CBF-02D0BAF2941E}" name="intitule" dataDxfId="30"/>
@@ -975,13 +978,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C57DFD-1CB4-4BB6-806B-B3A954B7C9AD}">
-  <dimension ref="A1:AF23"/>
+  <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1005,194 +1008,135 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="R1" t="s">
         <v>49</v>
       </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
         <v>50</v>
       </c>
-      <c r="O1" t="s">
+      <c r="T1" t="s">
         <v>51</v>
       </c>
-      <c r="P1" t="s">
+      <c r="U1" t="s">
         <v>52</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="V1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W1" t="s">
+        <v>54</v>
+      </c>
+      <c r="X1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="R1" t="s">
-        <v>53</v>
-      </c>
-      <c r="S1" t="s">
-        <v>54</v>
-      </c>
-      <c r="T1" t="s">
-        <v>55</v>
-      </c>
-      <c r="U1" t="s">
-        <v>56</v>
-      </c>
-      <c r="V1" t="s">
-        <v>57</v>
-      </c>
-      <c r="W1" t="s">
-        <v>58</v>
-      </c>
-      <c r="X1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" ht="288" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="11">
-        <v>77</v>
-      </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="W2" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="X2" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y2" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z2" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA2" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB2" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="AC2" s="11"/>
-      <c r="AD2" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="AE2" s="11" t="s">
-        <v>76</v>
-      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1222,18 +1166,18 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="1"/>
+      <c r="D4" s="2"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="2"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="K4" s="8"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -1243,12 +1187,12 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
+      <c r="U4" s="8"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
+      <c r="Z4" s="8"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
@@ -1280,39 +1224,98 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
+    <row r="6" spans="1:32" ht="288" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="11">
+        <v>77</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q6" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="S6" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="U6" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="V6" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="X6" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA6" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB6" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE6" s="11" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1340,105 +1343,45 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:32" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="O8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="U8" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y8" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z8" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA8" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB8" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AC8" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AD8" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="3"/>
+      <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1492,7 +1435,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1514,7 +1457,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
-      <c r="V11" s="6"/>
+      <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
@@ -1522,7 +1465,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1552,7 +1495,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1582,7 +1525,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1612,7 +1555,7 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1642,7 +1585,7 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1670,9 +1613,9 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1700,39 +1643,99 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U18" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z18" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD18" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="1"/>
-      <c r="X18" s="1"/>
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1760,9 +1763,9 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1784,15 +1787,15 @@
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
+      <c r="V20" s="6"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1820,9 +1823,9 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1850,9 +1853,9 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1880,6 +1883,36 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
complète les infos du suivi castor
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DCF4A5-9CD4-476C-8D28-E0FA6745BD18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981AA85C-6BC8-4C4E-9974-E18F0EED5AA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="7656" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="135">
   <si>
     <t>onde</t>
   </si>
@@ -437,54 +437,106 @@
     <t>texte:Le réseau castor;lien:https://professionnels.ofb.fr/fr/reseau-castor</t>
   </si>
   <si>
+    <t>https://carmen.carmencarto.fr/38/Castor.map</t>
+  </si>
+  <si>
+    <t>texte:Fiche espèce;lien:https://professionnels.ofb.fr/fr/doc-fiches-especes/castor-deurope-castor-fiber</t>
+  </si>
+  <si>
+    <t>Les objectifs du réseau ont été fixés par le ministère en charge de l’écologie :
+- assurer le suivi de la colonisation du castor sur le réseau hydrographique français ;
+- accompagnement sur la question des dommages;
+- vigilance sur l'arrivée du castor canadien</t>
+  </si>
+  <si>
+    <t>Raportage Directive européenne Habitat Faune Flore
+Régulation des dispositifs de piègeage près des cours d'eau</t>
+  </si>
+  <si>
+    <t>Prospection de linéaires de cours d'eau à la recherche d'indices de présence</t>
+  </si>
+  <si>
+    <t>data-raw/logo_castor.jpg</t>
+  </si>
+  <si>
+    <t>Baguage
+Ecoute des mâles chanteurs (qui croulent)
+Suivi de l'habitat</t>
+  </si>
+  <si>
+    <t>data-raw/lineaire_castor.gpkg</t>
+  </si>
+  <si>
+    <t>77, 91</t>
+  </si>
+  <si>
+    <t>Coordination
+Remontée des données au national</t>
+  </si>
+  <si>
+    <t>Recherche d'indices de présence (bois coupé, écorçage, hutte…) en prospection sur l'eau et à pied en berge</t>
+  </si>
+  <si>
+    <t>texte: Site Alfresco du Réseau Castor IdF;lien:https://ged.ofb.fr/share/page/site/dridf-rseau-partenarial-castor/dashboard</t>
+  </si>
+  <si>
+    <t>texte: Protocole;lien:https://ged.ofb.fr/share/s/giB4EPFIRPmsQZiGFeYY0A</t>
+  </si>
+  <si>
+    <t>- embarquation (ex. kayak)
+- gilet de sauvetage
+- jumelles
+- appareil photo
+- GPS</t>
+  </si>
+  <si>
+    <t>Quasi disparu en Europe au début du 20ème siècle, la prise de mesure de protection du Castor d’Europe à partir de 1909 puis son classement en « espèce protégée » en 1968 a permis leur reconquête du territoire. L’ Ile-de-France est l’un des fronts de colonisation, induisant un suivi annuel et précis permettant de détecter la présence, suivre la distribution de l’espèce et la protéger en conséquence (notamment via l’interdiction de piégeage).</t>
+  </si>
+  <si>
+    <t>Prospections préférentiellement hivernales avant la reprise de la végétation</t>
+  </si>
+  <si>
     <t>Animation nationale:
 Paul Hurel
 Suivi scientifique:
 Yoann Bressan
+Couriel du réseau:
+reseau.castor@ofb.gouv.fr
 Animation régionale:
 Cédric Mondy</t>
   </si>
   <si>
-    <t>ENS
+    <t>Conseils départementaux (ENS)
 Syndicats de rivière</t>
   </si>
   <si>
-    <t>https://carmen.carmencarto.fr/38/Castor.map</t>
-  </si>
-  <si>
-    <t>texte:Fiche espèce;lien:https://professionnels.ofb.fr/fr/doc-fiches-especes/castor-deurope-castor-fiber</t>
-  </si>
-  <si>
-    <t>Le Castor d'Europe est un mammifère semi-aquatique, et l'un des plus grand rongeur de la planète.
-Cette espèce protégée est une "ingénieure des écosystèmes" au travers des différents aménagements qu'elle réalise dans les cours d'eau.</t>
-  </si>
-  <si>
-    <t>Les objectifs du réseau ont été fixés par le ministère en charge de l’écologie :
-- assurer le suivi de la colonisation du castor sur le réseau hydrographique français ;
-- accompagnement sur la question des dommages;
-- vigilance sur l'arrivée du castor canadien</t>
-  </si>
-  <si>
-    <t>Raportage Directive européenne Habitat Faune Flore
-Régulation des dispositifs de piègeage près des cours d'eau</t>
-  </si>
-  <si>
-    <t>Prospection de linéaires de cours d'eau à la recherche d'indices de présence</t>
-  </si>
-  <si>
-    <t>data-raw/logo_castor.jpg</t>
-  </si>
-  <si>
-    <t>Baguage
-Ecoute des mâles chanteurs (qui croulent)
-Suivi de l'habitat</t>
+    <t>environ 1/2 journée par prospection</t>
+  </si>
+  <si>
+    <t>4j</t>
+  </si>
+  <si>
+    <t>Formation Petit et Méso-Carnivores et Castor
+(Formation dommage)</t>
+  </si>
+  <si>
+    <t>Prospections
+(Constats de dommage)</t>
+  </si>
+  <si>
+    <t>Remplissage des fiches terrains
+Bancarisation régionale
+Transmission au national qui effectue une validation et consolidation nationale des données</t>
+  </si>
+  <si>
+    <t>texte:Arrêtés piégeage (Serveur DR);lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\Castor\04_ArretesPiegeage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -512,21 +564,45 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FFD9E1F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -564,13 +640,13 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1028,33 +1104,33 @@
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="11.44140625" style="4"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" customWidth="1"/>
-    <col min="6" max="6" width="25.88671875" customWidth="1"/>
-    <col min="7" max="10" width="15.6640625" customWidth="1"/>
+    <col min="1" max="3" width="11.42578125" style="4"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="7" max="10" width="15.7109375" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="21.33203125" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" customWidth="1"/>
-    <col min="14" max="14" width="15.5546875" customWidth="1"/>
-    <col min="18" max="19" width="14.88671875" customWidth="1"/>
-    <col min="20" max="21" width="20.88671875" customWidth="1"/>
-    <col min="22" max="22" width="38.5546875" customWidth="1"/>
+    <col min="12" max="12" width="21.28515625" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" customWidth="1"/>
+    <col min="18" max="19" width="14.85546875" customWidth="1"/>
+    <col min="20" max="21" width="20.85546875" customWidth="1"/>
+    <col min="22" max="22" width="38.5703125" customWidth="1"/>
     <col min="24" max="24" width="16" customWidth="1"/>
-    <col min="25" max="25" width="18.109375" customWidth="1"/>
-    <col min="27" max="29" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.140625" customWidth="1"/>
+    <col min="27" max="29" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
@@ -1152,7 +1228,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -1182,7 +1258,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:32" ht="288" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" ht="195" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -1190,59 +1266,92 @@
         <v>109</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G3" s="1">
-        <v>91</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K3" s="1"/>
+      <c r="K3" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="L3" s="1" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
+      <c r="O3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="W3" s="8" t="s">
+        <v>124</v>
+      </c>
       <c r="X3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Y3" s="1"/>
+      <c r="Y3" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="Z3" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="AA3" s="1" t="s">
         <v>110</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>103</v>
       </c>
@@ -1272,7 +1381,7 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="8"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -1302,73 +1411,73 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:32" ht="288" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" ht="330" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="F6" s="11" t="s">
+      <c r="E6" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="10">
         <v>77</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12" t="s">
+      <c r="H6" s="10"/>
+      <c r="I6" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="M6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11" t="s">
+      <c r="N6" s="10"/>
+      <c r="O6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="P6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="Q6" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="R6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="S6" s="11" t="s">
+      <c r="S6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="T6" s="11" t="s">
+      <c r="T6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="U6" s="11" t="s">
+      <c r="U6" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="V6" s="12" t="s">
+      <c r="V6" s="11" t="s">
         <v>97</v>
       </c>
       <c r="W6" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="X6" s="11" t="s">
+      <c r="X6" s="10" t="s">
         <v>36</v>
       </c>
       <c r="Y6" s="7" t="s">
@@ -1377,21 +1486,21 @@
       <c r="Z6" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="AA6" s="11" t="s">
+      <c r="AA6" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="AB6" s="11" t="s">
+      <c r="AB6" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="11" t="s">
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="AE6" s="11" t="s">
+      <c r="AE6" s="10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -1421,7 +1530,7 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
@@ -1451,7 +1560,7 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>104</v>
       </c>
@@ -1481,7 +1590,7 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1511,7 +1620,7 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -1541,7 +1650,7 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -1571,7 +1680,7 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
@@ -1601,7 +1710,7 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
@@ -1631,7 +1740,7 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
@@ -1661,7 +1770,7 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>107</v>
       </c>
@@ -1691,7 +1800,7 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>105</v>
       </c>
@@ -1721,7 +1830,7 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:30" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" ht="210" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>0</v>
       </c>
@@ -1811,7 +1920,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
@@ -1841,7 +1950,7 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>106</v>
       </c>
@@ -1871,7 +1980,7 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>16</v>
       </c>
@@ -1901,7 +2010,7 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
@@ -1931,7 +2040,7 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>7</v>
       </c>
@@ -1961,7 +2070,7 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
ajoute les infos loup
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981AA85C-6BC8-4C4E-9974-E18F0EED5AA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEF59D8-C934-436E-B41C-6CD2D112377B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="160">
   <si>
     <t>onde</t>
   </si>
@@ -530,6 +530,106 @@
   </si>
   <si>
     <t>texte:Arrêtés piégeage (Serveur DR);lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\Castor\04_ArretesPiegeage</t>
+  </si>
+  <si>
+    <t>Réseau Loup/lynx</t>
+  </si>
+  <si>
+    <t>Logo-xl-reseau-Loup-lynx-558x374.jpg (558×374) (loupfrance.fr)</t>
+  </si>
+  <si>
+    <t>Espèce protégée depuis 1979 par la convention de Berne et recolonisant petit à petit le pays, le loup gris est encore très peu présent  en Ile-de-France. Le réseau Loup est déployé au niveau « Sentinelle » depuis 2017, et différentes procédures peuvent être mise en place en cas de signalement ou de détection d’un individu.</t>
+  </si>
+  <si>
+    <t>Veille, constats de dommages, observations opportunistes et prospections.</t>
+  </si>
+  <si>
+    <t>Les données sont valorisées dans les flash infos loup, dans les bilans saisonniers et annuels. Cela permet d’avoir une connaissance sur la population de loups et son aire de répartition et d’accompagner les acteurs et victimes éventuelles.</t>
+  </si>
+  <si>
+    <t>75,77,78,91,92,93,94,95</t>
+  </si>
+  <si>
+    <t>Opportuniste</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7,8,9,10,11,12</t>
+  </si>
+  <si>
+    <t>Sur signalement</t>
+  </si>
+  <si>
+    <t>Animation nationale:
+Nicolas Jean
+Animation régionale:
+Samuel Dembski
+Courriel du réseau:
+reseau.loup-lynx@ofb.gouv.fr</t>
+  </si>
+  <si>
+    <t>DRIEAT/DDT
+Préfecture</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>Base de données
+Synthèse
+Harmonisation des protocoles</t>
+  </si>
+  <si>
+    <t>Centralisation
+Formation
+Analyse de signalement</t>
+  </si>
+  <si>
+    <t>Constats
+Suivi
+Prélèvements</t>
+  </si>
+  <si>
+    <t>- Formation constat de dommage (1,5 jours)
+- Formation correspondant de réseau ( 3 jours)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 fiches de signalement, dites « fiches indices » sont disponibles. Chaque fiche est liée à un type d’évènement signalé (observation visuelle, photo, empreintes et piste, excrément/poils, hurlement, cadavre de proie sauvage, cadavre de proie domestique, urine/sang, cadavre
+Si prélèvement de matériel biologique, stockage dans un congélateur spécifique. Eviter la congélation/décongélation de l’ADN. Délai de 48h maximum après l’évènement pour des analyses de cadavres.
+</t>
+  </si>
+  <si>
+    <t>Selon la situation, plusieurs choses peuvent être nécessaires  (voir matériel détaillé pour chaque cas): 
+Fiche adaptée
+Appareil photo et GPS
+Si présence d’un cadavre: 
+Gants, scalpel, sac de récupération d’indice, feutre indélébile
+Housse mortuaire
+Masque, gel hydroalcoolique
+Prendre systématiquement le kit matériel complet et l’ensemble des fiches du réseau pour tout signalement.</t>
+  </si>
+  <si>
+    <t>SAGIR</t>
+  </si>
+  <si>
+    <t>- Réception du témoignage et prise de contact.
+- Compléter la ou les fiches indices adéquates et fournir une carte de localisation (1/25000ème), si possible des coordonnées GPS en Lambert 93 et tout élément pertinent (photo, vidéo, échantillons).
+- Transmettre cela à l’animateur régional du réseau et au service Connaissance de la Direction Régionale.
+- Analyse et classement de l’évènement, transmission des résultats à la DDT.</t>
+  </si>
+  <si>
+    <t>https://www.loupfrance.fr</t>
+  </si>
+  <si>
+    <t>texte:Guide réflexe (serveur DR);lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\Loup\Guide réflexe réseau Loup Lynx_DRIDF_v2.3.pdf</t>
+  </si>
+  <si>
+    <t>texte: Kit nouveaux territoires (serveur DR):lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\Loup\01_Documentation\KIT_Nouveaux_Territoires.pdf</t>
+  </si>
+  <si>
+    <t>texte:Fiches de signalement;lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\Loup</t>
+  </si>
+  <si>
+    <t>texte: Plan loup;lien:https://agriculture.gouv.fr/plan-loup-un-nouveau-cadre-national-dactions-pour-renforcer-la-coexistence-du-loup-et-des-activites</t>
   </si>
 </sst>
 </file>
@@ -610,7 +710,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -648,6 +748,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1104,10 +1205,10 @@
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="V5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC3" sqref="AC3"/>
+      <selection pane="bottomRight" activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,8 +1225,9 @@
     <col min="18" max="19" width="14.85546875" customWidth="1"/>
     <col min="20" max="21" width="20.85546875" customWidth="1"/>
     <col min="22" max="22" width="38.5703125" customWidth="1"/>
+    <col min="23" max="23" width="29" customWidth="1"/>
     <col min="24" max="24" width="16" customWidth="1"/>
-    <col min="25" max="25" width="18.140625" customWidth="1"/>
+    <col min="25" max="25" width="29.85546875" customWidth="1"/>
     <col min="27" max="29" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="32" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
@@ -1381,37 +1483,95 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="8"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" ht="285" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="B5" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-    </row>
-    <row r="6" spans="1:32" ht="330" x14ac:dyDescent="0.25">
+      <c r="O5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="U5" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y5" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" ht="255" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
@@ -2101,10 +2261,13 @@
       <c r="Z24" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" display="https://www.loupfrance.fr/wp-content/uploads/Logo-xl-reseau-Loup-lynx-558x374.jpg" xr:uid="{27C333FC-2187-470A-9EAE-03AF18F8C27F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@abd951765935790977bbbd957c83274f16cc08e0 🚀
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981AA85C-6BC8-4C4E-9974-E18F0EED5AA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEF59D8-C934-436E-B41C-6CD2D112377B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="160">
   <si>
     <t>onde</t>
   </si>
@@ -530,6 +530,106 @@
   </si>
   <si>
     <t>texte:Arrêtés piégeage (Serveur DR);lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\Castor\04_ArretesPiegeage</t>
+  </si>
+  <si>
+    <t>Réseau Loup/lynx</t>
+  </si>
+  <si>
+    <t>Logo-xl-reseau-Loup-lynx-558x374.jpg (558×374) (loupfrance.fr)</t>
+  </si>
+  <si>
+    <t>Espèce protégée depuis 1979 par la convention de Berne et recolonisant petit à petit le pays, le loup gris est encore très peu présent  en Ile-de-France. Le réseau Loup est déployé au niveau « Sentinelle » depuis 2017, et différentes procédures peuvent être mise en place en cas de signalement ou de détection d’un individu.</t>
+  </si>
+  <si>
+    <t>Veille, constats de dommages, observations opportunistes et prospections.</t>
+  </si>
+  <si>
+    <t>Les données sont valorisées dans les flash infos loup, dans les bilans saisonniers et annuels. Cela permet d’avoir une connaissance sur la population de loups et son aire de répartition et d’accompagner les acteurs et victimes éventuelles.</t>
+  </si>
+  <si>
+    <t>75,77,78,91,92,93,94,95</t>
+  </si>
+  <si>
+    <t>Opportuniste</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7,8,9,10,11,12</t>
+  </si>
+  <si>
+    <t>Sur signalement</t>
+  </si>
+  <si>
+    <t>Animation nationale:
+Nicolas Jean
+Animation régionale:
+Samuel Dembski
+Courriel du réseau:
+reseau.loup-lynx@ofb.gouv.fr</t>
+  </si>
+  <si>
+    <t>DRIEAT/DDT
+Préfecture</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>Base de données
+Synthèse
+Harmonisation des protocoles</t>
+  </si>
+  <si>
+    <t>Centralisation
+Formation
+Analyse de signalement</t>
+  </si>
+  <si>
+    <t>Constats
+Suivi
+Prélèvements</t>
+  </si>
+  <si>
+    <t>- Formation constat de dommage (1,5 jours)
+- Formation correspondant de réseau ( 3 jours)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 fiches de signalement, dites « fiches indices » sont disponibles. Chaque fiche est liée à un type d’évènement signalé (observation visuelle, photo, empreintes et piste, excrément/poils, hurlement, cadavre de proie sauvage, cadavre de proie domestique, urine/sang, cadavre
+Si prélèvement de matériel biologique, stockage dans un congélateur spécifique. Eviter la congélation/décongélation de l’ADN. Délai de 48h maximum après l’évènement pour des analyses de cadavres.
+</t>
+  </si>
+  <si>
+    <t>Selon la situation, plusieurs choses peuvent être nécessaires  (voir matériel détaillé pour chaque cas): 
+Fiche adaptée
+Appareil photo et GPS
+Si présence d’un cadavre: 
+Gants, scalpel, sac de récupération d’indice, feutre indélébile
+Housse mortuaire
+Masque, gel hydroalcoolique
+Prendre systématiquement le kit matériel complet et l’ensemble des fiches du réseau pour tout signalement.</t>
+  </si>
+  <si>
+    <t>SAGIR</t>
+  </si>
+  <si>
+    <t>- Réception du témoignage et prise de contact.
+- Compléter la ou les fiches indices adéquates et fournir une carte de localisation (1/25000ème), si possible des coordonnées GPS en Lambert 93 et tout élément pertinent (photo, vidéo, échantillons).
+- Transmettre cela à l’animateur régional du réseau et au service Connaissance de la Direction Régionale.
+- Analyse et classement de l’évènement, transmission des résultats à la DDT.</t>
+  </si>
+  <si>
+    <t>https://www.loupfrance.fr</t>
+  </si>
+  <si>
+    <t>texte:Guide réflexe (serveur DR);lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\Loup\Guide réflexe réseau Loup Lynx_DRIDF_v2.3.pdf</t>
+  </si>
+  <si>
+    <t>texte: Kit nouveaux territoires (serveur DR):lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\Loup\01_Documentation\KIT_Nouveaux_Territoires.pdf</t>
+  </si>
+  <si>
+    <t>texte:Fiches de signalement;lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\Loup</t>
+  </si>
+  <si>
+    <t>texte: Plan loup;lien:https://agriculture.gouv.fr/plan-loup-un-nouveau-cadre-national-dactions-pour-renforcer-la-coexistence-du-loup-et-des-activites</t>
   </si>
 </sst>
 </file>
@@ -610,7 +710,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -648,6 +748,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1104,10 +1205,10 @@
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="V5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC3" sqref="AC3"/>
+      <selection pane="bottomRight" activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,8 +1225,9 @@
     <col min="18" max="19" width="14.85546875" customWidth="1"/>
     <col min="20" max="21" width="20.85546875" customWidth="1"/>
     <col min="22" max="22" width="38.5703125" customWidth="1"/>
+    <col min="23" max="23" width="29" customWidth="1"/>
     <col min="24" max="24" width="16" customWidth="1"/>
-    <col min="25" max="25" width="18.140625" customWidth="1"/>
+    <col min="25" max="25" width="29.85546875" customWidth="1"/>
     <col min="27" max="29" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="32" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
@@ -1381,37 +1483,95 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="8"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" ht="285" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="B5" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-    </row>
-    <row r="6" spans="1:32" ht="330" x14ac:dyDescent="0.25">
+      <c r="O5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="U5" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y5" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" ht="255" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
@@ -2101,10 +2261,13 @@
       <c r="Z24" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" display="https://www.loupfrance.fr/wp-content/uploads/Logo-xl-reseau-Loup-lynx-558x374.jpg" xr:uid="{27C333FC-2187-470A-9EAE-03AF18F8C27F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajoute onepf et bocage
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEF59D8-C934-436E-B41C-6CD2D112377B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271E6708-A9C3-46A1-9A8D-BA7CE3FD2052}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="195">
   <si>
     <t>onde</t>
   </si>
@@ -470,6 +470,9 @@
     <t>77, 91</t>
   </si>
   <si>
+    <t>Prospections</t>
+  </si>
+  <si>
     <t>Coordination
 Remontée des données au national</t>
   </si>
@@ -535,9 +538,6 @@
     <t>Réseau Loup/lynx</t>
   </si>
   <si>
-    <t>Logo-xl-reseau-Loup-lynx-558x374.jpg (558×374) (loupfrance.fr)</t>
-  </si>
-  <si>
     <t>Espèce protégée depuis 1979 par la convention de Berne et recolonisant petit à petit le pays, le loup gris est encore très peu présent  en Ile-de-France. Le réseau Loup est déployé au niveau « Sentinelle » depuis 2017, et différentes procédures peuvent être mise en place en cas de signalement ou de détection d’un individu.</t>
   </si>
   <si>
@@ -591,11 +591,6 @@
   <si>
     <t>- Formation constat de dommage (1,5 jours)
 - Formation correspondant de réseau ( 3 jours)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9 fiches de signalement, dites « fiches indices » sont disponibles. Chaque fiche est liée à un type d’évènement signalé (observation visuelle, photo, empreintes et piste, excrément/poils, hurlement, cadavre de proie sauvage, cadavre de proie domestique, urine/sang, cadavre
-Si prélèvement de matériel biologique, stockage dans un congélateur spécifique. Eviter la congélation/décongélation de l’ADN. Délai de 48h maximum après l’évènement pour des analyses de cadavres.
-</t>
   </si>
   <si>
     <t>Selon la situation, plusieurs choses peuvent être nécessaires  (voir matériel détaillé pour chaque cas): 
@@ -623,13 +618,164 @@
     <t>texte:Guide réflexe (serveur DR);lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\Loup\Guide réflexe réseau Loup Lynx_DRIDF_v2.3.pdf</t>
   </si>
   <si>
-    <t>texte: Kit nouveaux territoires (serveur DR):lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\Loup\01_Documentation\KIT_Nouveaux_Territoires.pdf</t>
-  </si>
-  <si>
     <t>texte:Fiches de signalement;lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\Loup</t>
   </si>
   <si>
     <t>texte: Plan loup;lien:https://agriculture.gouv.fr/plan-loup-un-nouveau-cadre-national-dactions-pour-renforcer-la-coexistence-du-loup-et-des-activites</t>
+  </si>
+  <si>
+    <t>https://www.loupfrance.fr/wp-content/uploads/Logo-xl-reseau-Loup-lynx-558x374.jpg</t>
+  </si>
+  <si>
+    <t>Observatoire National de l’écosystème prairie de fauche</t>
+  </si>
+  <si>
+    <t>L’ONEPF a été crée avec le constat que les périodes de fenaisons de plus en plus précoces et l’altération des prairies de fauches sont défavorables aux nombreuses d’oiseaux qui l’utilisent pour la reproduction.</t>
+  </si>
+  <si>
+    <t>Suivi de l’avifaune prairiale et de l’évolution de la gestion des prairies de fauche. Echantillonnage de référence nationale. Etude de l’impact de la fauche sur les populations d’avifaune prairiale.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orientation des politiques publiques agro –environnementales, programmes de recherche, études complémentaires. </t>
+  </si>
+  <si>
+    <t>Stations d’une aire de 200m autour d’un point de la prairie de fauche (environ 12 ha chacun.)</t>
+  </si>
+  <si>
+    <t>Calendrier fenaison:6,7
+IPA:4,5,6
+Relevé de végétation:5,7</t>
+  </si>
+  <si>
+    <t>Tous les ans: 
+- Relevés des calendriers de fenaison :  évaluation du pourcentage fauché. 20 juin, 1er juillet, 15 juillet (+- 2 jours).
+- Comptage visuel et auditif des oiseaux : Indice ponctuel d’abondance (IPA), 2 fois.
+Tous les 5 ans: 
+Relevés de végétation et enquête agricole .</t>
+  </si>
+  <si>
+    <t>Animation nationale:
+xxxx
+Suivi scientifique:
+Laurence Curtet
+Animation régionale:
+Samuel Dembski</t>
+  </si>
+  <si>
+    <t>Fédération de chasse
+LPO</t>
+  </si>
+  <si>
+    <t>Animation</t>
+  </si>
+  <si>
+    <t>Prospection
+Saisie des données</t>
+  </si>
+  <si>
+    <t>- Bulletin de liaison de l'ONEPF
+- Articles scientifiques</t>
+  </si>
+  <si>
+    <t>Général:
+- Fiches de terrain
+- jumelles
+Relevés de végétation:
+- Mètre
+- Quadrillage</t>
+  </si>
+  <si>
+    <t>texte:PNA Outarde canepière (2020-2029);lien:https://outardecanepetiere.fr/le-plan-national-d-actions/le-3e-plan-national-d-actions-2020-2029</t>
+  </si>
+  <si>
+    <t>texte: Protocole et fiches (Serveur DR);lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\ONEPF\01_Documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La méthode retenue est celle des Indices Ponctuels d’Abondance (I.P.A.), adaptée ici au cas 
+particulier des oiseaux prairiaux qui sont mieux détectables visuellement que les oiseaux forestiers. 
+Cette méthode est surtout orientée vers l’échantillonnage des peuplements de passereaux
+Le nombre d’individus par espèce est recensé par un observateur immobile, au centre de chaque station, pendant une durée de 15 minutes. 
+Les oiseaux sont repérés soit à la jumelle, soit par leurs cris ou leurs chants. 
+Le recensement en un même point est à réaliser deux fois chaque année, dans la première puis la seconde moitié de la saison de nidification (avant la fenaison). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 fiches de signalement, dites « fiches indices » sont disponibles. Chaque fiche est liée à un type d’évènement signalé (observation visuelle, photo, empreintes et piste, excrément/poils, hurlement, cadavre de proie sauvage, cadavre de proie domestique, urine/sang, cadavre)
+Si prélèvement de matériel biologique, stockage dans un congélateur spécifique. Eviter la congélation/décongélation de l’ADN. Délai de 48h maximum après l’évènement pour des analyses de cadavres.
+</t>
+  </si>
+  <si>
+    <t>texte: Kit nouveaux territoires (serveur DR);lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\Loup\01_Documentation\KIT_Nouveaux_Territoires.pdf</t>
+  </si>
+  <si>
+    <t>Dispositif national de suivi des bocages</t>
+  </si>
+  <si>
+    <t>Le bocage est un paysage verdoyant de parcelles délimitées par des haies vives. De nombreux bocages ont disparus après la seconde guerre mondiale avec de grandes opérations de remembrement. Cependant, les haies et bocages sont des milieux privilégiés par de nombreuses espèces, et des facteurs de continuité écologique. Les deux premières phases du suivi ont été réalisées en 2020 avec la création d’une cartographie des territoires bocagers sur l’échelle de la France. Un protocole de suivi qualitatif et un référentiel national des haies sont maintenant développés pour les différents types de bocages.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relevés sur le terrain pour caractériser les haies. </t>
+  </si>
+  <si>
+    <t>Suivi de l’évolution des haies et bocages. Aide pour les documents de planification, politiques agricoles. Cibler les zones pour la mise en place de mesures de restauration. Promouvoir la gestion durable des milieux bocagers.</t>
+  </si>
+  <si>
+    <t>Quadrats de 1km²</t>
+  </si>
+  <si>
+    <t>Possible:1,2,3,4,5,6,7,8,9,10,11,12
+Préférable:5,6,7,8,9</t>
+  </si>
+  <si>
+    <t>Animation nationale:
+Sophie Morin
+Animation régionale:
+Samuel Dembski</t>
+  </si>
+  <si>
+    <t>IGN</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Animation
+Base de données</t>
+  </si>
+  <si>
+    <t>- Connaissance en botanique
+- Connaissance en ornithologie</t>
+  </si>
+  <si>
+    <t>Protocole national de relevé qualitatif  des haies. 
+A l’échelle d’un carré ou quadrat de 1 km².
+- Localisation des haies, des alignements d’arbres et des différents types d’occupation du sol présents
+- Description de l’état des fonctionnalités écologiques des haies : épaisseur, présence de bande enherbée, de bois mort, de lianes, micros-habitats, diversité d’essences, état sanitaire des végétaux, etc.</t>
+  </si>
+  <si>
+    <t>- Le fond orthophoto du carré fourni 
+- Un support rigide pour fixer les documents de terrain et un stylo 
+- Les fiches de description des haies du carré à l’échelle de 1km²
+- Un smartphone pour se repérer si nécessaire et faire de la prise de vue 
+- Télémètre
+- Guide botanique
+- Fiche de terrain</t>
+  </si>
+  <si>
+    <t>- relevés de terrain
+- Transmission des fiches</t>
+  </si>
+  <si>
+    <t>https://www.geoportail.gouv.fr
+https://geoservices.ign.fr/bdhaie</t>
+  </si>
+  <si>
+    <t>texte:Présentation du dispositif;lien:http://www.set-revue.fr/caracteriser-et-suivre-qualitativement-et-quantitativement-les-haies-et-le-bocage-en-France</t>
+  </si>
+  <si>
+    <t>texte:Plaquette d'information;lien:http://www.polebocage.fr/IMG/pdf/dsb_4pages_v11.pdf</t>
+  </si>
+  <si>
+    <t>texte:Atlas des densités de haies;lien:https://ged.ofb.fr/share/page/site/ple-bocage-faune-sauvage</t>
   </si>
 </sst>
 </file>
@@ -710,7 +856,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -749,6 +895,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1205,10 +1357,10 @@
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="V5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W5" sqref="W5"/>
+      <selection pane="bottomRight" activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,7 +1370,7 @@
     <col min="5" max="5" width="23.42578125" customWidth="1"/>
     <col min="6" max="6" width="25.85546875" customWidth="1"/>
     <col min="7" max="10" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" customWidth="1"/>
     <col min="12" max="12" width="21.28515625" customWidth="1"/>
     <col min="13" max="13" width="13.85546875" customWidth="1"/>
     <col min="14" max="14" width="15.5703125" customWidth="1"/>
@@ -1371,7 +1523,7 @@
         <v>116</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>113</v>
@@ -1392,47 +1544,47 @@
         <v>108</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>33</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="T3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="U3" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="V3" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W3" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Z3" s="1" t="s">
         <v>111</v>
@@ -1444,13 +1596,13 @@
         <v>112</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AF3" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
@@ -1488,10 +1640,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>137</v>
@@ -1544,31 +1696,31 @@
         <v>150</v>
       </c>
       <c r="V5" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="W5" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="X5" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="Y5" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="Y5" s="8" t="s">
+      <c r="Z5" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="AA5" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AD5" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AA5" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AE5" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AF5" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="AE5" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="AF5" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:32" ht="255" x14ac:dyDescent="0.25">
@@ -1690,35 +1842,75 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" ht="285" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="14" t="s">
+        <v>159</v>
+      </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G8" s="1">
+        <v>77</v>
+      </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
+      <c r="P8" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
+      <c r="R8" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>169</v>
+      </c>
       <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
+      <c r="V8" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="W8" s="8" t="s">
+        <v>171</v>
+      </c>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
+      <c r="Z8" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -2170,35 +2362,84 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" ht="255" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>177</v>
+      </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
+      <c r="I22" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
+      <c r="L22" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>184</v>
+      </c>
       <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
+      <c r="O22" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="U22" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="W22" s="8" t="s">
+        <v>189</v>
+      </c>
       <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
+      <c r="Y22" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="Z22" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="AC22" s="1" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -2262,7 +2503,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" display="https://www.loupfrance.fr/wp-content/uploads/Logo-xl-reseau-Loup-lynx-558x374.jpg" xr:uid="{27C333FC-2187-470A-9EAE-03AF18F8C27F}"/>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{27C333FC-2187-470A-9EAE-03AF18F8C27F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@e4066a77f40164ec693446f3f893ef5b741c0a9c 🚀
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEF59D8-C934-436E-B41C-6CD2D112377B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943E925A-092D-49AD-80EF-2DC87622F03D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="195">
   <si>
     <t>onde</t>
   </si>
@@ -470,6 +470,9 @@
     <t>77, 91</t>
   </si>
   <si>
+    <t>Prospections</t>
+  </si>
+  <si>
     <t>Coordination
 Remontée des données au national</t>
   </si>
@@ -535,9 +538,6 @@
     <t>Réseau Loup/lynx</t>
   </si>
   <si>
-    <t>Logo-xl-reseau-Loup-lynx-558x374.jpg (558×374) (loupfrance.fr)</t>
-  </si>
-  <si>
     <t>Espèce protégée depuis 1979 par la convention de Berne et recolonisant petit à petit le pays, le loup gris est encore très peu présent  en Ile-de-France. Le réseau Loup est déployé au niveau « Sentinelle » depuis 2017, et différentes procédures peuvent être mise en place en cas de signalement ou de détection d’un individu.</t>
   </si>
   <si>
@@ -591,11 +591,6 @@
   <si>
     <t>- Formation constat de dommage (1,5 jours)
 - Formation correspondant de réseau ( 3 jours)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9 fiches de signalement, dites « fiches indices » sont disponibles. Chaque fiche est liée à un type d’évènement signalé (observation visuelle, photo, empreintes et piste, excrément/poils, hurlement, cadavre de proie sauvage, cadavre de proie domestique, urine/sang, cadavre
-Si prélèvement de matériel biologique, stockage dans un congélateur spécifique. Eviter la congélation/décongélation de l’ADN. Délai de 48h maximum après l’évènement pour des analyses de cadavres.
-</t>
   </si>
   <si>
     <t>Selon la situation, plusieurs choses peuvent être nécessaires  (voir matériel détaillé pour chaque cas): 
@@ -623,13 +618,164 @@
     <t>texte:Guide réflexe (serveur DR);lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\Loup\Guide réflexe réseau Loup Lynx_DRIDF_v2.3.pdf</t>
   </si>
   <si>
-    <t>texte: Kit nouveaux territoires (serveur DR):lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\Loup\01_Documentation\KIT_Nouveaux_Territoires.pdf</t>
-  </si>
-  <si>
     <t>texte:Fiches de signalement;lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\Loup</t>
   </si>
   <si>
     <t>texte: Plan loup;lien:https://agriculture.gouv.fr/plan-loup-un-nouveau-cadre-national-dactions-pour-renforcer-la-coexistence-du-loup-et-des-activites</t>
+  </si>
+  <si>
+    <t>https://www.loupfrance.fr/wp-content/uploads/Logo-xl-reseau-Loup-lynx-558x374.jpg</t>
+  </si>
+  <si>
+    <t>Observatoire National de l’écosystème prairie de fauche</t>
+  </si>
+  <si>
+    <t>L’ONEPF a été crée avec le constat que les périodes de fenaisons de plus en plus précoces et l’altération des prairies de fauches sont défavorables aux nombreuses d’oiseaux qui l’utilisent pour la reproduction.</t>
+  </si>
+  <si>
+    <t>Suivi de l’avifaune prairiale et de l’évolution de la gestion des prairies de fauche. Echantillonnage de référence nationale. Etude de l’impact de la fauche sur les populations d’avifaune prairiale.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orientation des politiques publiques agro –environnementales, programmes de recherche, études complémentaires. </t>
+  </si>
+  <si>
+    <t>Stations d’une aire de 200m autour d’un point de la prairie de fauche (environ 12 ha chacun.)</t>
+  </si>
+  <si>
+    <t>Calendrier fenaison:6,7
+IPA:4,5,6
+Relevé de végétation:5,7</t>
+  </si>
+  <si>
+    <t>Tous les ans: 
+- Relevés des calendriers de fenaison :  évaluation du pourcentage fauché. 20 juin, 1er juillet, 15 juillet (+- 2 jours).
+- Comptage visuel et auditif des oiseaux : Indice ponctuel d’abondance (IPA), 2 fois.
+Tous les 5 ans: 
+Relevés de végétation et enquête agricole .</t>
+  </si>
+  <si>
+    <t>Animation nationale:
+xxxx
+Suivi scientifique:
+Laurence Curtet
+Animation régionale:
+Samuel Dembski</t>
+  </si>
+  <si>
+    <t>Fédération de chasse
+LPO</t>
+  </si>
+  <si>
+    <t>Animation</t>
+  </si>
+  <si>
+    <t>Prospection
+Saisie des données</t>
+  </si>
+  <si>
+    <t>- Bulletin de liaison de l'ONEPF
+- Articles scientifiques</t>
+  </si>
+  <si>
+    <t>Général:
+- Fiches de terrain
+- jumelles
+Relevés de végétation:
+- Mètre
+- Quadrillage</t>
+  </si>
+  <si>
+    <t>texte:PNA Outarde canepière (2020-2029);lien:https://outardecanepetiere.fr/le-plan-national-d-actions/le-3e-plan-national-d-actions-2020-2029</t>
+  </si>
+  <si>
+    <t>texte: Protocole et fiches (Serveur DR);lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\ONEPF\01_Documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La méthode retenue est celle des Indices Ponctuels d’Abondance (I.P.A.), adaptée ici au cas 
+particulier des oiseaux prairiaux qui sont mieux détectables visuellement que les oiseaux forestiers. 
+Cette méthode est surtout orientée vers l’échantillonnage des peuplements de passereaux
+Le nombre d’individus par espèce est recensé par un observateur immobile, au centre de chaque station, pendant une durée de 15 minutes. 
+Les oiseaux sont repérés soit à la jumelle, soit par leurs cris ou leurs chants. 
+Le recensement en un même point est à réaliser deux fois chaque année, dans la première puis la seconde moitié de la saison de nidification (avant la fenaison). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 fiches de signalement, dites « fiches indices » sont disponibles. Chaque fiche est liée à un type d’évènement signalé (observation visuelle, photo, empreintes et piste, excrément/poils, hurlement, cadavre de proie sauvage, cadavre de proie domestique, urine/sang, cadavre)
+Si prélèvement de matériel biologique, stockage dans un congélateur spécifique. Eviter la congélation/décongélation de l’ADN. Délai de 48h maximum après l’évènement pour des analyses de cadavres.
+</t>
+  </si>
+  <si>
+    <t>texte: Kit nouveaux territoires (serveur DR);lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\Loup\01_Documentation\KIT_Nouveaux_Territoires.pdf</t>
+  </si>
+  <si>
+    <t>Dispositif national de suivi des bocages</t>
+  </si>
+  <si>
+    <t>Le bocage est un paysage verdoyant de parcelles délimitées par des haies vives. De nombreux bocages ont disparus après la seconde guerre mondiale avec de grandes opérations de remembrement. Cependant, les haies et bocages sont des milieux privilégiés par de nombreuses espèces, et des facteurs de continuité écologique. Les deux premières phases du suivi ont été réalisées en 2020 avec la création d’une cartographie des territoires bocagers sur l’échelle de la France. Un protocole de suivi qualitatif et un référentiel national des haies sont maintenant développés pour les différents types de bocages.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relevés sur le terrain pour caractériser les haies. </t>
+  </si>
+  <si>
+    <t>Suivi de l’évolution des haies et bocages. Aide pour les documents de planification, politiques agricoles. Cibler les zones pour la mise en place de mesures de restauration. Promouvoir la gestion durable des milieux bocagers.</t>
+  </si>
+  <si>
+    <t>Quadrats de 1km²</t>
+  </si>
+  <si>
+    <t>Possible:1,2,3,4,5,6,7,8,9,10,11,12
+Préférable:5,6,7,8,9</t>
+  </si>
+  <si>
+    <t>Animation nationale:
+Sophie Morin
+Animation régionale:
+Samuel Dembski</t>
+  </si>
+  <si>
+    <t>IGN</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Animation
+Base de données</t>
+  </si>
+  <si>
+    <t>- Connaissance en botanique
+- Connaissance en ornithologie</t>
+  </si>
+  <si>
+    <t>Protocole national de relevé qualitatif  des haies. 
+A l’échelle d’un carré ou quadrat de 1 km².
+- Localisation des haies, des alignements d’arbres et des différents types d’occupation du sol présents
+- Description de l’état des fonctionnalités écologiques des haies : épaisseur, présence de bande enherbée, de bois mort, de lianes, micros-habitats, diversité d’essences, état sanitaire des végétaux, etc.</t>
+  </si>
+  <si>
+    <t>- Le fond orthophoto du carré fourni 
+- Un support rigide pour fixer les documents de terrain et un stylo 
+- Les fiches de description des haies du carré à l’échelle de 1km²
+- Un smartphone pour se repérer si nécessaire et faire de la prise de vue 
+- Télémètre
+- Guide botanique
+- Fiche de terrain</t>
+  </si>
+  <si>
+    <t>- relevés de terrain
+- Transmission des fiches</t>
+  </si>
+  <si>
+    <t>https://www.geoportail.gouv.fr
+https://geoservices.ign.fr/bdhaie</t>
+  </si>
+  <si>
+    <t>texte:Présentation du dispositif;lien:http://www.set-revue.fr/caracteriser-et-suivre-qualitativement-et-quantitativement-les-haies-et-le-bocage-en-France</t>
+  </si>
+  <si>
+    <t>texte:Plaquette d'information;lien:http://www.polebocage.fr/IMG/pdf/dsb_4pages_v11.pdf</t>
+  </si>
+  <si>
+    <t>texte:Atlas des densités de haies;lien:https://ged.ofb.fr/share/page/site/ple-bocage-faune-sauvage</t>
   </si>
 </sst>
 </file>
@@ -710,7 +856,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -749,6 +895,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1205,10 +1357,10 @@
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="V5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="T19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W5" sqref="W5"/>
+      <selection pane="bottomRight" activeCell="AD22" sqref="AD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,7 +1370,7 @@
     <col min="5" max="5" width="23.42578125" customWidth="1"/>
     <col min="6" max="6" width="25.85546875" customWidth="1"/>
     <col min="7" max="10" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" customWidth="1"/>
     <col min="12" max="12" width="21.28515625" customWidth="1"/>
     <col min="13" max="13" width="13.85546875" customWidth="1"/>
     <col min="14" max="14" width="15.5703125" customWidth="1"/>
@@ -1371,7 +1523,7 @@
         <v>116</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>113</v>
@@ -1392,47 +1544,47 @@
         <v>108</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>33</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="T3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="U3" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="V3" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W3" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Z3" s="1" t="s">
         <v>111</v>
@@ -1444,13 +1596,13 @@
         <v>112</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AF3" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
@@ -1488,10 +1640,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>137</v>
@@ -1544,31 +1696,31 @@
         <v>150</v>
       </c>
       <c r="V5" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="W5" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="X5" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="Y5" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="Y5" s="8" t="s">
+      <c r="Z5" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="AA5" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AD5" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AA5" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AE5" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AF5" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="AE5" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="AF5" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:32" ht="255" x14ac:dyDescent="0.25">
@@ -1690,35 +1842,75 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" ht="285" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="14" t="s">
+        <v>159</v>
+      </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G8" s="1">
+        <v>77</v>
+      </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
+      <c r="P8" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
+      <c r="R8" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>169</v>
+      </c>
       <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
+      <c r="V8" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="W8" s="8" t="s">
+        <v>171</v>
+      </c>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
+      <c r="Z8" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -2170,35 +2362,82 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" ht="255" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>177</v>
+      </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
+      <c r="I22" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
+      <c r="L22" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>184</v>
+      </c>
       <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
+      <c r="O22" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
+      <c r="R22" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="U22" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="W22" s="8" t="s">
+        <v>189</v>
+      </c>
       <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
+      <c r="Y22" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="Z22" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="AC22" s="1" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -2262,7 +2501,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" display="https://www.loupfrance.fr/wp-content/uploads/Logo-xl-reseau-Loup-lynx-558x374.jpg" xr:uid="{27C333FC-2187-470A-9EAE-03AF18F8C27F}"/>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{27C333FC-2187-470A-9EAE-03AF18F8C27F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@8ef821e046db366c32d9568c245c5f16d2f31778 🚀
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943E925A-092D-49AD-80EF-2DC87622F03D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271E6708-A9C3-46A1-9A8D-BA7CE3FD2052}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="195">
   <si>
     <t>onde</t>
   </si>
@@ -1357,10 +1357,10 @@
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="T19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD22" sqref="AD22"/>
+      <selection pane="bottomRight" activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2403,7 +2403,9 @@
       <c r="P22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Q22" s="1"/>
+      <c r="Q22" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="R22" s="1" t="s">
         <v>186</v>
       </c>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@2b895efdb26f2f9be9bf52ad0cc449399985e874 🚀
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271E6708-A9C3-46A1-9A8D-BA7CE3FD2052}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A91F020-DE44-4587-B2BB-1662D6DD33DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="216">
   <si>
     <t>onde</t>
   </si>
@@ -230,12 +230,6 @@
 - Cartes de densité</t>
   </si>
   <si>
-    <t>temps_formation</t>
-  </si>
-  <si>
-    <t>2-3j</t>
-  </si>
-  <si>
     <t>Carte de bagueur (formation spécifique et plus de 10 soirées de baguage encadrées)
 Reconnaissance chants</t>
   </si>
@@ -295,9 +289,6 @@
   <si>
     <t>- Suivi usuel: 1 fois par mois, le 25 (+/- 2 jours)
 - Suivi complémentaire: potentiellement toute l'année, en fonction des conditions hydrologiques</t>
-  </si>
-  <si>
-    <t>1j</t>
   </si>
   <si>
     <t>Initié</t>
@@ -516,9 +507,6 @@
     <t>environ 1/2 journée par prospection</t>
   </si>
   <si>
-    <t>4j</t>
-  </si>
-  <si>
     <t>Formation Petit et Méso-Carnivores et Castor
 (Formation dommage)</t>
   </si>
@@ -776,6 +764,103 @@
   </si>
   <si>
     <t>texte:Atlas des densités de haies;lien:https://ged.ofb.fr/share/page/site/ple-bocage-faune-sauvage</t>
+  </si>
+  <si>
+    <t>Caractérisation hydromorphologique des cours d’eau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’hydromorphologie des cours d’eau est une des composante majeure de son état de santé. Ces caractéristiques dépendent des conditions naturelles et paysagères et peuvent être altérées par les activités humaines. Carhyce est le protocole de recueil de données hydromorphologiques à l'échelle d’une station sur les cours d'eau prospectables à pied. Les données sont standardisées et comparables dans le temps et d’un site à l’autre. </t>
+  </si>
+  <si>
+    <t>Relever les caractéristiques morphologique du cours d’eau au travers de différents ateliers : Définition de la station ; Granulométrie ; Pente de la ligne d’eau ; Débit ; Transects ; Caractérisation de la zone riparienne ; Colmatage…</t>
+  </si>
+  <si>
+    <t>Quantifier l'altération hydromorphologique des cours d'eau. Orienter les mesures de gestion. Définir un cadre de travail lors d'opérations de restauration.</t>
+  </si>
+  <si>
+    <t>75, 77, 78, 91, 92, 93, 94, 95</t>
+  </si>
+  <si>
+    <t>Stations des réseaux DCE
+Sites suivis dans le cadre d'opérations de restauration</t>
+  </si>
+  <si>
+    <t>5,6,7,8,9</t>
+  </si>
+  <si>
+    <t>Pour les stations DCE: tout les 6 ans
+Les relevés sont à effectuer en période d'étiage</t>
+  </si>
+  <si>
+    <t>Animation nationale:
+Karl Kreutzenberger
+Animation régionale:
+Samuel Dembski</t>
+  </si>
+  <si>
+    <t>DRIEAT/DDT
+Agence de l'eau</t>
+  </si>
+  <si>
+    <t>1/2j</t>
+  </si>
+  <si>
+    <t>nombre_agents</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>Relevés de terrain</t>
+  </si>
+  <si>
+    <t>Formation Carhyce  pour la mise en œuvre du protocole et la saisie des données dans l’application – 3 j</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obligatoire
+- Appareil photo, Barre à mine , Bâtonnets , Clinomètre , Courantomètre , GPS , Gabarit , Jalons-repères , Mires , Masse ou massette 
+Niveau à bulle, mire à bulles et trépied, Pied à coulisse ou réglet, Piquets métalliques , Planche et crayon , Ruban de mesure (30 m) , Télémètre , Topofil et bobine.
+- Matériel hygiène et sécurité
+- Fiche de recueil
+Optionnel
+Calculatrice , Machette , Règle de maçon à bulle , Talkies-walkies (paire) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Définition de la station (Appréciation visuelle du cours d’eau, géolocalisation, précise évaluation des grandeurs caractéristiques).
+Granulométrie (Mesure de 100 éléments sur le radier présentant la granulométrie la plus grossière). 
+Pente de la ligne d’eau (Mesure du denivelé entre le niveau d’eau à l’amont et à l’aval de la station avec au moins 3 points intermédiaires).
+Débit. 
+Transects  (Matérialisation de 15 transects perpendiculaires à l’écoulement, espacés de la largeur à plein bord).
+Colmatage  (Appréhender l’intensité du colmatage). </t>
+  </si>
+  <si>
+    <t>Naïades:
+https://naiades.eaufrance.fr/acces-donnees#/hydromorphologie
+Interface d'Exploitation des Données Carhyce:
+https://analytics.huma-num.fr/ied_carhyce/</t>
+  </si>
+  <si>
+    <t>texte:Plaquette de présentation;lien:https://professionnels.ofb.fr/sites/default/files/GP2017_Carhyce_Plaquette.pdf</t>
+  </si>
+  <si>
+    <t>texte:Vidéo de présentation;lien:https://www.dailymotion.com/video/x4ij5lc</t>
+  </si>
+  <si>
+    <t>texte:Protocole;lien:https://www.documentation.eauetbiodiversite.fr/notice/carhyce-caracterisation-hydromorphologique-des-cours-d-eau-protocole-de-recueil-de-donnees-hydromorp0</t>
+  </si>
+  <si>
+    <t>texte:Fiches Méthodologiques (serveur DR);lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\Hydromorphologie\Cours_Eau[CarHyCE]\01_Documentation</t>
+  </si>
+  <si>
+    <t>- Relevés des données sur le terrain
+- Saisie des données dans l’application web Carhyce (https://carhyce.eaufrance.fr/)
+Tous les 6 mois, les données migrent vers la plateforme IED (Interface d’Exploitation des Données), où elles sont traitées et mises en forme, permettant leur visualisation sous forme de graphiques.</t>
+  </si>
+  <si>
+    <t>https://carhyce.eaufrance.fr/images/icone_carhyce.png</t>
   </si>
 </sst>
 </file>
@@ -856,7 +941,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -901,6 +986,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -926,6 +1017,9 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
@@ -951,9 +1045,6 @@
     </dxf>
     <dxf>
       <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
@@ -1036,22 +1127,22 @@
     <tableColumn id="10" xr3:uid="{2F64F147-A984-4D54-83A0-29F317643399}" name="transversalite" dataDxfId="18"/>
     <tableColumn id="11" xr3:uid="{29D5CB78-6BB9-49AD-A55A-A97CA9799332}" name="duree" dataDxfId="17"/>
     <tableColumn id="12" xr3:uid="{869EED11-E2FC-46E0-ACF9-0DDC82CE3DC4}" name="expertise" dataDxfId="16"/>
-    <tableColumn id="28" xr3:uid="{A3E722CE-A375-4AE8-9CF3-1282C439126B}" name="temps_formation" dataDxfId="15"/>
-    <tableColumn id="13" xr3:uid="{F4DBE069-BA7F-4080-94B2-8ABBF7538774}" name="role_national" dataDxfId="14"/>
-    <tableColumn id="14" xr3:uid="{258750F9-2A96-4283-887D-9CFA4D17F439}" name="role_regional" dataDxfId="13"/>
-    <tableColumn id="15" xr3:uid="{9871871F-54ED-487E-A03C-7A8C48D3CFC5}" name="role_departemental" dataDxfId="12"/>
-    <tableColumn id="24" xr3:uid="{FD209E5E-CC51-404C-B64E-C171238903FA}" name="droits_formations" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{199EAB2D-1AF2-4CDB-8DA8-9AFCF50D2515}" name="protocole" dataDxfId="10"/>
-    <tableColumn id="17" xr3:uid="{98D077C8-A3ED-4384-B70C-4A4280C26FE7}" name="materiel" dataDxfId="9"/>
-    <tableColumn id="18" xr3:uid="{5054FBBA-5094-4C33-92F7-7A30AFA38A22}" name="autres_releves" dataDxfId="8"/>
-    <tableColumn id="19" xr3:uid="{FD214916-9E0C-4234-853A-5FE7AF8CF557}" name="saisie_validation" dataDxfId="7"/>
-    <tableColumn id="20" xr3:uid="{214FE337-1EDA-4253-A78D-B9247E4FADAF}" name="diffusion" dataDxfId="6"/>
-    <tableColumn id="21" xr3:uid="{D5A66587-DDDF-4D32-897E-51F4D17676D7}" name="plus_recto1" dataDxfId="5"/>
-    <tableColumn id="29" xr3:uid="{68D7BF7D-E5CC-41EC-90C5-AF11729CC6D2}" name="plus_recto2" dataDxfId="4"/>
-    <tableColumn id="30" xr3:uid="{5A2652F8-BC92-4FC4-A98C-E430D61980AA}" name="plus_recto3" dataDxfId="3"/>
-    <tableColumn id="27" xr3:uid="{9293E153-542E-44B7-8608-6A7DF028B0AB}" name="plus_verso1" dataDxfId="2"/>
-    <tableColumn id="31" xr3:uid="{03BAB4B1-56CF-43A6-AFEC-CB2C3A01FBC2}" name="plus_verso2" dataDxfId="1"/>
-    <tableColumn id="32" xr3:uid="{A8A25170-2E24-4434-9B14-0CA372542DEF}" name="plus_verso3" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{C4310D48-97B0-4BC5-8D16-B16809824F9D}" name="nombre_agents" dataDxfId="0"/>
+    <tableColumn id="13" xr3:uid="{F4DBE069-BA7F-4080-94B2-8ABBF7538774}" name="role_national" dataDxfId="15"/>
+    <tableColumn id="14" xr3:uid="{258750F9-2A96-4283-887D-9CFA4D17F439}" name="role_regional" dataDxfId="14"/>
+    <tableColumn id="15" xr3:uid="{9871871F-54ED-487E-A03C-7A8C48D3CFC5}" name="role_departemental" dataDxfId="13"/>
+    <tableColumn id="24" xr3:uid="{FD209E5E-CC51-404C-B64E-C171238903FA}" name="droits_formations" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{199EAB2D-1AF2-4CDB-8DA8-9AFCF50D2515}" name="protocole" dataDxfId="11"/>
+    <tableColumn id="17" xr3:uid="{98D077C8-A3ED-4384-B70C-4A4280C26FE7}" name="materiel" dataDxfId="10"/>
+    <tableColumn id="18" xr3:uid="{5054FBBA-5094-4C33-92F7-7A30AFA38A22}" name="autres_releves" dataDxfId="9"/>
+    <tableColumn id="19" xr3:uid="{FD214916-9E0C-4234-853A-5FE7AF8CF557}" name="saisie_validation" dataDxfId="8"/>
+    <tableColumn id="20" xr3:uid="{214FE337-1EDA-4253-A78D-B9247E4FADAF}" name="diffusion" dataDxfId="7"/>
+    <tableColumn id="21" xr3:uid="{D5A66587-DDDF-4D32-897E-51F4D17676D7}" name="plus_recto1" dataDxfId="6"/>
+    <tableColumn id="29" xr3:uid="{68D7BF7D-E5CC-41EC-90C5-AF11729CC6D2}" name="plus_recto2" dataDxfId="5"/>
+    <tableColumn id="30" xr3:uid="{5A2652F8-BC92-4FC4-A98C-E430D61980AA}" name="plus_recto3" dataDxfId="4"/>
+    <tableColumn id="27" xr3:uid="{9293E153-542E-44B7-8608-6A7DF028B0AB}" name="plus_verso1" dataDxfId="3"/>
+    <tableColumn id="31" xr3:uid="{03BAB4B1-56CF-43A6-AFEC-CB2C3A01FBC2}" name="plus_verso2" dataDxfId="2"/>
+    <tableColumn id="32" xr3:uid="{A8A25170-2E24-4434-9B14-0CA372542DEF}" name="plus_verso3" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1357,10 +1448,10 @@
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q23" sqref="Q23"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,6 +1465,7 @@
     <col min="12" max="12" width="21.28515625" customWidth="1"/>
     <col min="13" max="13" width="13.85546875" customWidth="1"/>
     <col min="14" max="14" width="15.5703125" customWidth="1"/>
+    <col min="17" max="17" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="14.85546875" customWidth="1"/>
     <col min="20" max="21" width="20.85546875" customWidth="1"/>
     <col min="22" max="22" width="38.5703125" customWidth="1"/>
@@ -1410,7 +1502,7 @@
         <v>42</v>
       </c>
       <c r="I1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J1" t="s">
         <v>43</v>
@@ -1419,7 +1511,7 @@
         <v>44</v>
       </c>
       <c r="L1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M1" t="s">
         <v>45</v>
@@ -1434,7 +1526,7 @@
         <v>48</v>
       </c>
       <c r="Q1" t="s">
-        <v>63</v>
+        <v>202</v>
       </c>
       <c r="R1" t="s">
         <v>49</v>
@@ -1464,22 +1556,22 @@
         <v>57</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
@@ -1517,97 +1609,97 @@
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>131</v>
+      <c r="Q3" s="16" t="s">
+        <v>203</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>33</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="V3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="W3" s="8" t="s">
         <v>122</v>
-      </c>
-      <c r="W3" s="8" t="s">
-        <v>125</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="AF3" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1640,87 +1732,87 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Q5" s="1" t="s">
-        <v>64</v>
+      <c r="Q5" s="1">
+        <v>1</v>
       </c>
       <c r="R5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="U5" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="W5" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="X5" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="Y5" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="U5" s="8" t="s">
+      <c r="Z5" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="V5" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="W5" s="1" t="s">
+      <c r="AA5" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AD5" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="AE5" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AF5" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="Y5" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="AA5" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="AD5" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="AE5" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="AF5" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:32" ht="255" x14ac:dyDescent="0.25">
@@ -1731,13 +1823,13 @@
         <v>58</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>29</v>
@@ -1747,16 +1839,16 @@
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M6" s="10" t="s">
         <v>30</v>
@@ -1768,8 +1860,8 @@
       <c r="P6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="Q6" s="10" t="s">
-        <v>64</v>
+      <c r="Q6" s="17" t="s">
+        <v>204</v>
       </c>
       <c r="R6" s="10" t="s">
         <v>33</v>
@@ -1781,35 +1873,35 @@
         <v>35</v>
       </c>
       <c r="U6" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="V6" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="W6" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="X6" s="10" t="s">
         <v>36</v>
       </c>
       <c r="Y6" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Z6" s="7" t="s">
         <v>62</v>
       </c>
       <c r="AA6" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AB6" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AC6" s="10"/>
       <c r="AD6" s="10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="AE6" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
@@ -1847,74 +1939,76 @@
         <v>5</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G8" s="1">
         <v>77</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Q8" s="1"/>
+      <c r="Q8" s="1">
+        <v>1</v>
+      </c>
       <c r="R8" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>34</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="U8" s="1"/>
       <c r="V8" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="W8" s="8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="AD8" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -2124,7 +2218,7 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -2152,9 +2246,9 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2182,7 +2276,7 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:30" ht="210" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" ht="210" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>0</v>
       </c>
@@ -2190,13 +2284,13 @@
         <v>61</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>19</v>
@@ -2205,19 +2299,19 @@
         <v>20</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>28</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>25</v>
@@ -2227,10 +2321,10 @@
         <v>21</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>1</v>
       </c>
       <c r="R18" s="1" t="s">
         <v>22</v>
@@ -2242,10 +2336,10 @@
         <v>27</v>
       </c>
       <c r="U18" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="W18" s="1" t="s">
         <v>23</v>
@@ -2254,25 +2348,25 @@
         <v>24</v>
       </c>
       <c r="Y18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z18" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC18" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="Z18" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA18" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AB18" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AC18" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="AD18" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
@@ -2302,9 +2396,9 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -2332,116 +2426,174 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" ht="330" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="B21" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>195</v>
+      </c>
       <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
+      <c r="I21" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>200</v>
+      </c>
       <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
+      <c r="O21" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>5</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y21" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="AA21" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="AD21" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>213</v>
+      </c>
     </row>
-    <row r="22" spans="1:30" ht="255" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" ht="255" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="P22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Q22" s="1" t="s">
-        <v>84</v>
+      <c r="Q22" s="1">
+        <v>1</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="S22" s="1" t="s">
         <v>34</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="U22" s="8" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="W22" s="8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="X22" s="1"/>
       <c r="Y22" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z22" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AC22" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="Z22" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="AA22" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="AB22" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="AC22" s="1" t="s">
-        <v>194</v>
-      </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>7</v>
       </c>
@@ -2471,7 +2623,7 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@7d5250297ce5e4fc30b8a21bf104478aaabe5460 🚀
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A91F020-DE44-4587-B2BB-1662D6DD33DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296DB7C5-D4AC-487F-AF20-A947AED83BBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="238">
   <si>
     <t>onde</t>
   </si>
@@ -861,6 +861,105 @@
   </si>
   <si>
     <t>https://carhyce.eaufrance.fr/images/icone_carhyce.png</t>
+  </si>
+  <si>
+    <t>Suivi du chat forestier</t>
+  </si>
+  <si>
+    <t>Présent au sud et à l’est de l’Ile-de-France, le chat forestier est protégé depuis 1979. Son abondance et sa répartition sont étudiés dans le cadre du réseau PMCC. Cependant, des études plus spécifiques sont parfois menées, utilisant des pièges à des points définis.</t>
+  </si>
+  <si>
+    <t>Identifier les zones de présence de l'espèce et évaluer le degré d'hybridation avec le chat domestique</t>
+  </si>
+  <si>
+    <t>Les résultats des observations sont valorisés en cartes d’abondance et de répartition, articles scientifiques et rapports. Evaluation de l’état de conservation dans le cadre de la directive DHFF.</t>
+  </si>
+  <si>
+    <t>12,1,2,3</t>
+  </si>
+  <si>
+    <t>Relevés toutes les deux semaines pendant 3 mois</t>
+  </si>
+  <si>
+    <t>Animation nationale:
+Paul hurel
+Suivi scientifique:
+Yoann Bressan
+Sandrine Ruette
+Animateur régional:
+Cédric Mondy</t>
+  </si>
+  <si>
+    <t>Animation
+Validation des observations
+Analyses génétiques
+Base de données</t>
+  </si>
+  <si>
+    <t>Animation
+Valorisation</t>
+  </si>
+  <si>
+    <t>Prospections
+Recueil de signalement
+Saisie des données</t>
+  </si>
+  <si>
+    <t>Formation de 3 jours sur les petits et moyens carnivores et l'utilisation de l'outil rezo-pmcc</t>
+  </si>
+  <si>
+    <t>Secteurs d'étude d'environ 100km²  comprenant des lisières forestières au contact de prairies. 
+Chaque secteur est suivi par un minimum de six dispositifs</t>
+  </si>
+  <si>
+    <t>ONF
+ARB
+Conseils départementaux (ENS)
+Réserve de la Bassée
+Ile-de-France Nature
+CPIE Boucles de la Marne</t>
+  </si>
+  <si>
+    <t>Signalement de collision:
+- Récupération de tissus et envoi pour analyse
+Suivi pièges photographiques:
+- Pose de dispositifs (piège photo + piège à poil + attractif à base de valériane)
+- Relevés des photos et poils éventuels
+- Stérilisation du piège à poil et recharge en attractif</t>
+  </si>
+  <si>
+    <t>Signalement de collision:
+- kit de prélèvement PMCC (gants, tube Eppendorf, alcool, ciseaux)
+- fiche adaptée
+Suivi pièges photographiques:
+- pièges photographiques
+- brosses métalliques (pièges à poils)
+- attractif à base de valériane
+- gants, pinces à épiler, enveloppes
+- fiche adaptée</t>
+  </si>
+  <si>
+    <t>Saisie des observations sur l'application Rezo-PMCC (pour les observations annexes: saisie sur Rezo-PMCC ou Oison en fonction des espèces)
+Transmission des prélèvements à la DRAS pour analyses génétiques
+Validation des observations sur photo sur la base du phénotype</t>
+  </si>
+  <si>
+    <t>SINP national (https://openobs.mnhn.fr) ou régional (https://geonature.arb-idf.fr/geonature/)</t>
+  </si>
+  <si>
+    <t>texte:Fiche Espèce;lien:https://professionnels.ofb.fr/fr/doc-fiches-especes/chat-forestier-felis-silvestris-silvestris</t>
+  </si>
+  <si>
+    <t>texte:Plaquette de présentation de l'étude;lien:https://oai-gem.ofb.fr/exl-php/document-affiche/ofb_recherche_oai/OUVRE_DOC/49974?fic=doc00073302.pdf</t>
+  </si>
+  <si>
+    <t>texte:Site Alfresco de l'étude;lien:https://ged.ofb.fr/share/page/site/etude-chat-forestier-idf/dashboard</t>
+  </si>
+  <si>
+    <t>texte:Protocole;lien:https://ged.ofb.fr/share/s/sY4zG36QS1aDJ34fKNlrhw</t>
+  </si>
+  <si>
+    <t>texte:Vidéo en collaboration avec le MNHN;lien:https://youtu.be/UopppCJfUHA?feature=shared</t>
   </si>
 </sst>
 </file>
@@ -1448,10 +1547,10 @@
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1574,35 +1673,92 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" ht="225" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="C2" s="5"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G2" s="1">
+        <v>77.91</v>
+      </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>228</v>
+      </c>
       <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
+      <c r="O2" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>230</v>
+      </c>
       <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
+      <c r="Y2" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="3" spans="1:32" ht="195" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@7ad16f50a25c45c8e78b523eee348ae89b2740fe 🚀
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296DB7C5-D4AC-487F-AF20-A947AED83BBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF06483-47EF-41A3-88D4-C85D3540092B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="251">
   <si>
     <t>onde</t>
   </si>
@@ -960,6 +960,65 @@
   </si>
   <si>
     <t>texte:Vidéo en collaboration avec le MNHN;lien:https://youtu.be/UopppCJfUHA?feature=shared</t>
+  </si>
+  <si>
+    <t>Réseau Petits et méso-carnivores</t>
+  </si>
+  <si>
+    <t>75,77,78,95,91,94</t>
+  </si>
+  <si>
+    <t>Animation
+Formation</t>
+  </si>
+  <si>
+    <t>Observations
+Recueil de signalement
+Saisie des données</t>
+  </si>
+  <si>
+    <t>Articles de recherche
+Portail cartographique: https://professionnels.ofb.fr/fr/node/1089</t>
+  </si>
+  <si>
+    <t>texte: Documents sur les classements ESOD (serveur DR);lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\PMC\ESOD</t>
+  </si>
+  <si>
+    <t>texte:Page du réseau;lien:https://professionnels.ofb.fr/fr/reseau-petits-meso-carnivores</t>
+  </si>
+  <si>
+    <t>- Suivre l’évolution de l’aire de répartitions des 14 espèces, la dynamique de certaines populations et améliorer les connaissances sur leur écologie.
+- Former et partager les connaissances sur l’écologie de ces espèces.
+- Apporter une expertise technique et des conseils pour la gestion des espèces, évaluer la mise en œuvre des règlementations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Rapportages européens (DHFF, EEE)
+- Listes rouges de l'UICN
+- Classement 'Espèces susceptibles d'occasionner des dégâts (ESOD)'
+</t>
+  </si>
+  <si>
+    <t>Animation nationale:
+Paul Hurel
+Suivi scientifique:
+Yoann Bressan
+Référente technique:
+Laurence Henry
+Animateur régional:
+Cédric Mondy</t>
+  </si>
+  <si>
+    <t>Le réseau Petits et mésocarnivores (PMC) suit l’évolution de la répartition des populations de 14 espèces de carnivores en France métropolitaine, aux statuts règlementaires et de conservation variés. Les connaissances acquises grâce à ce réseau interne permettent à l’Office français de la biodiversité (OFB) d’apporter une expertise technique et scientifique sur ces espèces à tous les niveaux : départemental, régional, national et européen</t>
+  </si>
+  <si>
+    <t>En général:
+- Accès à l'outil Rezo-PMCC (appli smartphone ou site internet)
+Prélèvement tissu pour analyse génétique:
+- kit de prélèvement PMCC (gants, tube Eppendorf, alcool, ciseaux)
+- fiche adaptée</t>
+  </si>
+  <si>
+    <t>texte:Site de saisie Rezo-PMCC;lien:https://geo.ofb.fr/adws/app/a7e35981-0ec6-11eb-9154-93c04439bf0b/index.html</t>
   </si>
 </sst>
 </file>
@@ -1547,10 +1606,10 @@
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="V11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="AD17" sqref="AD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,8 +1749,8 @@
       <c r="F2" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="G2" s="1">
-        <v>77.91</v>
+      <c r="G2" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
@@ -2372,35 +2431,80 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" ht="255" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>238</v>
+      </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>239</v>
+      </c>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="I16" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>247</v>
+      </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
+      <c r="O16" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>1</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>226</v>
+      </c>
       <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
+      <c r="W16" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
+      <c r="Z16" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="AA16" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="AD16" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="AE16" s="1" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@9dc3be2757c2546159d15c989b1cd48ebdab29e4 🚀
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF06483-47EF-41A3-88D4-C85D3540092B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC51934-6DF5-45FE-AFA0-BEE6EF7A26C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="252">
   <si>
     <t>onde</t>
   </si>
@@ -965,9 +965,6 @@
     <t>Réseau Petits et méso-carnivores</t>
   </si>
   <si>
-    <t>75,77,78,95,91,94</t>
-  </si>
-  <si>
     <t>Animation
 Formation</t>
   </si>
@@ -1019,6 +1016,13 @@
   </si>
   <si>
     <t>texte:Site de saisie Rezo-PMCC;lien:https://geo.ofb.fr/adws/app/a7e35981-0ec6-11eb-9154-93c04439bf0b/index.html</t>
+  </si>
+  <si>
+    <t>Saisie des observations sur l'application Rezo-PMCC
+Pour les espèces d'identification délicate ou en limite/en dehors de leur aire de distribution: validation manuelle, utilisation possible de la génétique</t>
+  </si>
+  <si>
+    <t>75,77,78,95,91, 92,93,94</t>
   </si>
 </sst>
 </file>
@@ -1606,10 +1610,10 @@
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="V11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD17" sqref="AD17"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2440,16 +2444,16 @@
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E16" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="F16" s="8" t="s">
-        <v>246</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
@@ -2462,7 +2466,7 @@
         <v>137</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -2479,31 +2483,33 @@
         <v>182</v>
       </c>
       <c r="S16" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="T16" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="T16" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="U16" s="1" t="s">
         <v>226</v>
       </c>
       <c r="V16" s="1"/>
       <c r="W16" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="AA16" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="AD16" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1" t="s">
+      <c r="AE16" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="AA16" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="AD16" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="AE16" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@c84a1072c19e97812b686b421db507484ce9ba44 🚀
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC51934-6DF5-45FE-AFA0-BEE6EF7A26C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FB26A2-8706-43A3-AF1E-0D34C2267FC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -995,16 +995,6 @@
 </t>
   </si>
   <si>
-    <t>Animation nationale:
-Paul Hurel
-Suivi scientifique:
-Yoann Bressan
-Référente technique:
-Laurence Henry
-Animateur régional:
-Cédric Mondy</t>
-  </si>
-  <si>
     <t>Le réseau Petits et mésocarnivores (PMC) suit l’évolution de la répartition des populations de 14 espèces de carnivores en France métropolitaine, aux statuts règlementaires et de conservation variés. Les connaissances acquises grâce à ce réseau interne permettent à l’Office français de la biodiversité (OFB) d’apporter une expertise technique et scientifique sur ces espèces à tous les niveaux : départemental, régional, national et européen</t>
   </si>
   <si>
@@ -1023,6 +1013,16 @@
   </si>
   <si>
     <t>75,77,78,95,91, 92,93,94</t>
+  </si>
+  <si>
+    <t>Animation nationale:
+Paul Hurel
+Suivi scientifique:
+Yoann Bressan
+Référence technique:
+Laurence Henry
+Animation régionale:
+Cédric Mondy</t>
   </si>
 </sst>
 </file>
@@ -1613,7 +1613,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomRight" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2444,7 +2444,7 @@
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>244</v>
@@ -2453,7 +2453,7 @@
         <v>245</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
@@ -2466,7 +2466,7 @@
         <v>137</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -2493,11 +2493,11 @@
       </c>
       <c r="V16" s="1"/>
       <c r="W16" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="X16" s="1"/>
       <c r="Y16" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Z16" s="1" t="s">
         <v>241</v>
@@ -2506,7 +2506,7 @@
         <v>243</v>
       </c>
       <c r="AD16" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AE16" s="1" t="s">
         <v>242</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@7a537e4e662cc8c8cd3cc426ebeea9dd6cb80f3f 🚀
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FB26A2-8706-43A3-AF1E-0D34C2267FC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA33390F-9ACA-4F20-AABE-15048279B128}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="251">
   <si>
     <t>onde</t>
   </si>
@@ -1005,13 +1005,6 @@
 - fiche adaptée</t>
   </si>
   <si>
-    <t>texte:Site de saisie Rezo-PMCC;lien:https://geo.ofb.fr/adws/app/a7e35981-0ec6-11eb-9154-93c04439bf0b/index.html</t>
-  </si>
-  <si>
-    <t>Saisie des observations sur l'application Rezo-PMCC
-Pour les espèces d'identification délicate ou en limite/en dehors de leur aire de distribution: validation manuelle, utilisation possible de la génétique</t>
-  </si>
-  <si>
     <t>75,77,78,95,91, 92,93,94</t>
   </si>
   <si>
@@ -1023,6 +1016,10 @@
 Laurence Henry
 Animation régionale:
 Cédric Mondy</t>
+  </si>
+  <si>
+    <t>Saisie des observations sur l'application Rezo-PMCC (https://geo.ofb.fr/rezopmcc)
+Pour les espèces d'identification délicate ou en limite/en dehors de leur aire de distribution: validation manuelle, utilisation possible de la génétique</t>
   </si>
 </sst>
 </file>
@@ -1610,10 +1607,10 @@
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="V14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L16" sqref="L16"/>
+      <selection pane="bottomRight" activeCell="AD16" sqref="AD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2453,7 +2450,7 @@
         <v>245</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
@@ -2466,7 +2463,7 @@
         <v>137</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -2497,7 +2494,7 @@
       </c>
       <c r="X16" s="1"/>
       <c r="Y16" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="Z16" s="1" t="s">
         <v>241</v>
@@ -2506,9 +2503,6 @@
         <v>243</v>
       </c>
       <c r="AD16" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="AE16" s="1" t="s">
         <v>242</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@ae96c24532950728b6302bb65ebc7aa70008bb99 🚀
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA33390F-9ACA-4F20-AABE-15048279B128}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BBBC35-3419-4C87-B780-16936E12AFE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="270">
   <si>
     <t>onde</t>
   </si>
@@ -413,9 +413,6 @@
     <t>adne</t>
   </si>
   <si>
-    <t>continuites</t>
-  </si>
-  <si>
     <t>pmc</t>
   </si>
   <si>
@@ -1020,6 +1017,89 @@
   <si>
     <t>Saisie des observations sur l'application Rezo-PMCC (https://geo.ofb.fr/rezopmcc)
 Pour les espèces d'identification délicate ou en limite/en dehors de leur aire de distribution: validation manuelle, utilisation possible de la génétique</t>
+  </si>
+  <si>
+    <t>obstacles_ecoulement</t>
+  </si>
+  <si>
+    <t>Inventaire:1,2,3,4,5,6,7,8,9,10,11,12
+Hauteur de chute:5,6,7,8,9</t>
+  </si>
+  <si>
+    <t>Opportuniste ou plannifié
+A l'étiage pour la caractérisation des hauteurs de chute</t>
+  </si>
+  <si>
+    <t>Animation nationale: Karl Kreutzenberger
+Animation régionale:
+Cédric Mondy
+Assistance:
+assistance.geobs@ofb.gouv.fr</t>
+  </si>
+  <si>
+    <t>Agence de l'eau
+DRIEAT
+Syndicats de rivière
+Fédérations de pêche</t>
+  </si>
+  <si>
+    <t>Pratique</t>
+  </si>
+  <si>
+    <t>Coordination
+Contribution à l'évaluation des politiques publiques mises en place au niveau du bassin
+Formation</t>
+  </si>
+  <si>
+    <t>Animation locale
+Saisie
+Validation</t>
+  </si>
+  <si>
+    <t>Outil Géobs:
+- Consultation: sur demande
+- Saisie: Information dispensée par les agents de la DR
+- Validation: Correspondants continuité formés</t>
+  </si>
+  <si>
+    <t>Obstacles à l'Ecoulement</t>
+  </si>
+  <si>
+    <t>Collecter des informations objectives sur le nombre, la localisation et les caractéristiques des obstacles à l'écoulement sur les cours d'eau</t>
+  </si>
+  <si>
+    <t>Le ROE permet d’avoir une information spatialisée sur les obstacles à l’écoulement des cours d’eau d’origine humaine (caractéristiques, usages, gestion). Cette information peut être complétée dans la BDOE.</t>
+  </si>
+  <si>
+    <t>Elaboration d’un référentiel national et un socle commun d’information. Estimer la pression ouvrage sur les cours d'eau. 
+Suivi des politiques de restauration de la continuité écologique
+Calcul d’indicateurs de continuité écologique</t>
+  </si>
+  <si>
+    <t>Sandre:
+http://www.sandre.eaufrance.fr</t>
+  </si>
+  <si>
+    <t>- Fiche terrain
+- GPS
+- Appareil photo
+- Mire ou autre équipement permettant de mesurer la hauteur de chute</t>
+  </si>
+  <si>
+    <t>Saisie sur GéObs (https://geobs.eaufrance.fr/)
+Validation obligatoire par un agent de l'OFB disposant du profil validation</t>
+  </si>
+  <si>
+    <t>texte:Dataviz nationale;lien:https://professionnels.ofb.fr/fr/doc-dataviz/dataviz-mieux-connaitre-ouvrages-qui-jalonnent-nos-cours-deau</t>
+  </si>
+  <si>
+    <t>texte:Bilans (serveur DR);lien:\\ad.intra\dfs\COMMUNS\REGIONS\IDF\DR\05_CONNAISSANCE\ROE\04_Bilans</t>
+  </si>
+  <si>
+    <t>texte:La méthode ICE;lien:https://professionnels.ofb.fr/fr/node/387</t>
+  </si>
+  <si>
+    <t>texte:La continuité écologique des cours d'eau;lien:https://www.ofb.gouv.fr/la-continuite-ecologique-des-cours-deau</t>
   </si>
 </sst>
 </file>
@@ -1100,7 +1180,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1116,9 +1196,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1607,10 +1684,10 @@
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="V14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="U19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD16" sqref="AD16"/>
+      <selection pane="bottomRight" activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1685,7 +1762,7 @@
         <v>48</v>
       </c>
       <c r="Q1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="R1" t="s">
         <v>49</v>
@@ -1738,40 +1815,40 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>219</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>32</v>
@@ -1780,44 +1857,44 @@
         <v>1</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="U2" s="1" t="s">
-        <v>226</v>
-      </c>
       <c r="V2" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="W2" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="Z2" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD2" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="AC2" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="195" x14ac:dyDescent="0.25">
@@ -1825,92 +1902,92 @@
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="R3" s="10" t="s">
+      <c r="Q3" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="R3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="S3" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="T3" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="W3" s="8" t="s">
-        <v>122</v>
+      <c r="W3" s="7" t="s">
+        <v>121</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="Y3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF3" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="AF3" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
@@ -1926,7 +2003,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="8"/>
+      <c r="K4" s="7"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -1936,54 +2013,54 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-      <c r="U4" s="8"/>
+      <c r="U4" s="7"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="8"/>
+      <c r="Z4" s="7"/>
     </row>
     <row r="5" spans="1:32" ht="285" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>32</v>
@@ -1992,131 +2069,131 @@
         <v>1</v>
       </c>
       <c r="R5" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="U5" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="U5" s="8" t="s">
+      <c r="V5" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="W5" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="X5" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AE5" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="W5" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="Y5" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="AA5" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AF5" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="AE5" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="AF5" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:32" ht="255" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="E6" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="9">
         <v>77</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="11" t="s">
+      <c r="H6" s="9"/>
+      <c r="I6" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="M6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10" t="s">
+      <c r="N6" s="9"/>
+      <c r="O6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="P6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="Q6" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="R6" s="10" t="s">
+      <c r="Q6" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="R6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="S6" s="10" t="s">
+      <c r="S6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="T6" s="10" t="s">
+      <c r="T6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="U6" s="10" t="s">
+      <c r="U6" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="V6" s="11" t="s">
+      <c r="V6" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="W6" s="7" t="s">
+      <c r="W6" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="X6" s="10" t="s">
+      <c r="X6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="Y6" s="7" t="s">
+      <c r="Y6" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="Z6" s="7" t="s">
+      <c r="Z6" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="AA6" s="10" t="s">
+      <c r="AA6" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="AB6" s="10" t="s">
+      <c r="AB6" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="AC6" s="10"/>
-      <c r="AD6" s="10" t="s">
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="AE6" s="10" t="s">
+      <c r="AE6" s="9" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2154,37 +2231,37 @@
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>155</v>
+      <c r="B8" s="13" t="s">
+        <v>154</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="G8" s="1">
         <v>77</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -2195,31 +2272,31 @@
         <v>1</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>34</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="U8" s="1"/>
       <c r="V8" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="W8" s="8" t="s">
-        <v>167</v>
+        <v>169</v>
+      </c>
+      <c r="W8" s="7" t="s">
+        <v>166</v>
       </c>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
-      <c r="Z8" s="8" t="s">
-        <v>166</v>
+      <c r="Z8" s="7" t="s">
+        <v>165</v>
       </c>
       <c r="AA8" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AD8" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="AD8" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
@@ -2434,41 +2511,41 @@
     </row>
     <row r="16" spans="1:32" ht="255" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="E16" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="F16" s="8" t="s">
-        <v>245</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="K16" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>32</v>
@@ -2477,33 +2554,33 @@
         <v>1</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S16" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="T16" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="T16" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="U16" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V16" s="1"/>
       <c r="W16" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="X16" s="1"/>
       <c r="Y16" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Z16" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AA16" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="AD16" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="AA16" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="AD16" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
@@ -2567,7 +2644,7 @@
       <c r="J18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K18" s="8" t="s">
+      <c r="K18" s="7" t="s">
         <v>81</v>
       </c>
       <c r="L18" s="1" t="s">
@@ -2595,7 +2672,7 @@
       <c r="T18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U18" s="8" t="s">
+      <c r="U18" s="7" t="s">
         <v>83</v>
       </c>
       <c r="V18" s="1" t="s">
@@ -2610,7 +2687,7 @@
       <c r="Y18" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="Z18" s="8" t="s">
+      <c r="Z18" s="7" t="s">
         <v>85</v>
       </c>
       <c r="AA18" s="1" t="s">
@@ -2656,77 +2733,127 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" ht="165" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B20" s="5"/>
+        <v>250</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>259</v>
+      </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
+      <c r="J20" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>254</v>
+      </c>
       <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="6"/>
-      <c r="W20" s="1"/>
+      <c r="O20" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>1</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="V20" s="1"/>
+      <c r="W20" s="7" t="s">
+        <v>264</v>
+      </c>
       <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
+      <c r="Y20" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="AA20" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="AB20" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="AD20" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="AE20" s="1" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="21" spans="1:31" ht="330" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>32</v>
@@ -2735,43 +2862,43 @@
         <v>5</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="T21" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="U21" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="U21" s="1" t="s">
+      <c r="V21" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="W21" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="W21" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="X21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Y21" s="8" t="s">
-        <v>214</v>
+      <c r="Y21" s="7" t="s">
+        <v>213</v>
       </c>
       <c r="Z21" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="AA21" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="AA21" s="1" t="s">
+      <c r="AB21" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="AB21" s="1" t="s">
+      <c r="AD21" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="AD21" s="1" t="s">
+      <c r="AE21" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="AE21" s="1" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:31" ht="255" x14ac:dyDescent="0.25">
@@ -2779,38 +2906,38 @@
         <v>2</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="G22" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="M22" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P22" s="1" t="s">
         <v>32</v>
@@ -2819,38 +2946,38 @@
         <v>1</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S22" s="1" t="s">
         <v>34</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="U22" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="U22" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="V22" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="V22" s="1" t="s">
+      <c r="W22" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="W22" s="8" t="s">
+      <c r="X22" s="1"/>
+      <c r="Y22" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="8" t="s">
+      <c r="Z22" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="Z22" s="15" t="s">
+      <c r="AA22" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AA22" s="1" t="s">
+      <c r="AB22" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="AB22" s="1" t="s">
+      <c r="AC22" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="AC22" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@bf6c46802131977701aeb3800fa3da0e531c680a 🚀
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BBBC35-3419-4C87-B780-16936E12AFE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DAF35E-7D6D-4D21-979D-56F637C54210}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -1043,9 +1043,6 @@
 Fédérations de pêche</t>
   </si>
   <si>
-    <t>Pratique</t>
-  </si>
-  <si>
     <t>Coordination
 Contribution à l'évaluation des politiques publiques mises en place au niveau du bassin
 Formation</t>
@@ -1100,6 +1097,9 @@
   </si>
   <si>
     <t>texte:La continuité écologique des cours d'eau;lien:https://www.ofb.gouv.fr/la-continuite-ecologique-des-cours-deau</t>
+  </si>
+  <si>
+    <t>Formé</t>
   </si>
 </sst>
 </file>
@@ -1684,10 +1684,10 @@
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="U19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X20" sqref="X20"/>
+      <selection pane="bottomRight" activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2738,17 +2738,17 @@
         <v>250</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>262</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>135</v>
@@ -2772,7 +2772,7 @@
         <v>141</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="Q20" s="1">
         <v>1</v>
@@ -2781,36 +2781,36 @@
         <v>181</v>
       </c>
       <c r="S20" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="T20" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="T20" s="1" t="s">
+      <c r="U20" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>258</v>
       </c>
       <c r="V20" s="1"/>
       <c r="W20" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="X20" s="1"/>
       <c r="Y20" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="AA20" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="AB20" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="Z20" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="AA20" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="AB20" s="1" t="s">
+      <c r="AD20" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="AD20" s="1" t="s">
+      <c r="AE20" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="AE20" s="1" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="21" spans="1:31" ht="330" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@38be43384dd175127a53811e146b2f9f9759943b 🚀
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A2BCD5-3B1C-4590-AFD3-427BE8D4246F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747D6F9D-AD1B-47E2-B310-36F4A8FF6A8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -104,11 +104,6 @@
   <si>
     <t>Conseils départementaux
 DREAL</t>
-  </si>
-  <si>
-    <t>Pilotage
-Transmission
-Animation</t>
   </si>
   <si>
     <t>Observation
@@ -856,10 +851,6 @@
 Base de données</t>
   </si>
   <si>
-    <t>Animation
-Valorisation</t>
-  </si>
-  <si>
     <t>Prospections
 Recueil de signalement
 Saisie des données</t>
@@ -1006,11 +997,6 @@
 Fédérations de pêche</t>
   </si>
   <si>
-    <t>Coordination
-Contribution à l'évaluation des politiques publiques mises en place au niveau du bassin
-Formation</t>
-  </si>
-  <si>
     <t>Animation locale
 Saisie
 Validation</t>
@@ -1101,6 +1087,19 @@
 Kévin Le Rest
 Animation régionale:
 Samuel Dembski</t>
+  </si>
+  <si>
+    <t>Coordination
+Valorisation</t>
+  </si>
+  <si>
+    <t>Coordination
+Transmission</t>
+  </si>
+  <si>
+    <t>Coordination
+Interprétation
+Formation</t>
   </si>
 </sst>
 </file>
@@ -1688,7 +1687,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L21" sqref="L21"/>
+      <selection pane="bottomRight" activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1715,100 +1714,100 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>40</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>41</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" t="s">
         <v>42</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" t="s">
         <v>76</v>
       </c>
-      <c r="J1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>44</v>
       </c>
-      <c r="L1" t="s">
-        <v>77</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>45</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>46</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>47</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
+        <v>197</v>
+      </c>
+      <c r="R1" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" t="s">
-        <v>198</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>49</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>52</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>53</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>54</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>55</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>56</v>
       </c>
-      <c r="Z1" t="s">
-        <v>57</v>
-      </c>
       <c r="AA1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="225" x14ac:dyDescent="0.25">
@@ -1816,86 +1815,86 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="L2" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="1">
         <v>1</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="V2" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AA2" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AD2" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="195" x14ac:dyDescent="0.25">
@@ -1903,97 +1902,97 @@
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="S3" s="9" t="s">
+      <c r="V3" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="T3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="W3" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="Y3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AF3" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="AF3" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -2026,87 +2025,87 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q5" s="1">
         <v>1</v>
       </c>
       <c r="R5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="U5" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="U5" s="7" t="s">
+      <c r="V5" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="W5" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="X5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AE5" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="W5" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="Y5" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="AA5" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AF5" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="AE5" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="AF5" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:32" ht="255" x14ac:dyDescent="0.25">
@@ -2114,88 +2113,88 @@
         <v>1</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="9">
         <v>77</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N6" s="9"/>
       <c r="O6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="Q6" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="R6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="Q6" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="R6" s="9" t="s">
+      <c r="S6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="T6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="T6" s="9" t="s">
+      <c r="U6" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="V6" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="X6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="U6" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="V6" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="W6" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="X6" s="9" t="s">
-        <v>36</v>
-      </c>
       <c r="Y6" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Z6" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AA6" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB6" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="AB6" s="9" t="s">
-        <v>74</v>
       </c>
       <c r="AC6" s="9"/>
       <c r="AD6" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AE6" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
@@ -2233,76 +2232,76 @@
         <v>5</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="G8" s="1">
         <v>77</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q8" s="1">
         <v>1</v>
       </c>
       <c r="R8" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T8" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="U8" s="1"/>
       <c r="V8" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="W8" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AA8" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AD8" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="AD8" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -2512,81 +2511,81 @@
     </row>
     <row r="16" spans="1:32" ht="255" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="K16" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q16" s="1">
         <v>1</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="V16" s="1"/>
       <c r="W16" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="X16" s="1"/>
       <c r="Y16" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="Z16" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="AA16" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AA16" s="1" t="s">
-        <v>238</v>
-      </c>
       <c r="AD16" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2619,16 +2618,16 @@
         <v>0</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>19</v>
@@ -2637,19 +2636,19 @@
         <v>20</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="L18" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>25</v>
@@ -2659,7 +2658,7 @@
         <v>21</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q18" s="1">
         <v>1</v>
@@ -2668,16 +2667,16 @@
         <v>22</v>
       </c>
       <c r="S18" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="T18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T18" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="U18" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="W18" s="1" t="s">
         <v>23</v>
@@ -2686,22 +2685,22 @@
         <v>24</v>
       </c>
       <c r="Y18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z18" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="Z18" s="7" t="s">
+      <c r="AA18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD18" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="AA18" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AB18" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AC18" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AD18" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
@@ -2736,82 +2735,82 @@
     </row>
     <row r="20" spans="1:31" ht="165" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="Q20" s="1">
         <v>1</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>251</v>
+        <v>269</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="V20" s="1"/>
       <c r="W20" s="7" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="X20" s="1"/>
       <c r="Y20" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="AA20" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="AB20" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="AD20" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="AE20" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="Z20" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="AA20" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="AB20" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="AD20" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="AE20" s="1" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:31" ht="330" x14ac:dyDescent="0.25">
@@ -2819,87 +2818,87 @@
         <v>16</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q21" s="1">
         <v>5</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>160</v>
+        <v>33</v>
       </c>
       <c r="T21" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="U21" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="U21" s="1" t="s">
+      <c r="V21" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="W21" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="W21" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="X21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="Y21" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Z21" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="AA21" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="AA21" s="1" t="s">
+      <c r="AB21" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="AB21" s="1" t="s">
+      <c r="AD21" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="AD21" s="1" t="s">
+      <c r="AE21" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="AE21" s="1" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:31" ht="255" x14ac:dyDescent="0.25">
@@ -2907,78 +2906,78 @@
         <v>2</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="G22" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="M22" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q22" s="1">
         <v>1</v>
       </c>
       <c r="R22" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="U22" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="S22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="U22" s="7" t="s">
+      <c r="V22" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="V22" s="1" t="s">
+      <c r="W22" s="7" t="s">
         <v>180</v>
-      </c>
-      <c r="W22" s="7" t="s">
-        <v>181</v>
       </c>
       <c r="X22" s="1"/>
       <c r="Y22" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z22" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="Z22" s="14" t="s">
+      <c r="AA22" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="AA22" s="1" t="s">
+      <c r="AB22" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="AB22" s="1" t="s">
+      <c r="AC22" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="AC22" s="1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@fb9326c66aef425410cee426f7cca9cf7343327a 🚀
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23840CEC-0ACF-408D-AA6C-459CFC053D1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E49334-B43A-4F75-B0D7-FAFF26CCEE7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -1698,10 +1698,10 @@
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L17" sqref="L17"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@ced257e407426f00712ce22faad58ff758db52b5 🚀
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E49334-B43A-4F75-B0D7-FAFF26CCEE7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D747F6AE-D7BA-45AD-8131-3312C3A8CF07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -1075,18 +1075,6 @@
 reseau.becasse@ofb.gouv.fr</t>
   </si>
   <si>
-    <t>Animation nationale: Karl KREUTZENBERGER
-Animation régionale:
-Cédric MONDY
-Correspondants départementaux:
-PPC: Bérengère MONVOISIN
-77: Cyrille BOST
-78-95: Angélique EGLOFF
-91: Olivier MELART
-Assistance:
-assistance.geobs@ofb.gouv.fr</t>
-  </si>
-  <si>
     <t>Animation nationale:
 Paul HUREL
 Suivi scientifique:
@@ -1129,6 +1117,19 @@
 77: Anne-Gaëlle BLANC
 78-95: Amandine EVRARD
 91: Cyril KLEINPRINZ</t>
+  </si>
+  <si>
+    <t>Animation nationale: 
+Karl KREUTZENBERGER
+Animation régionale:
+Cédric MONDY
+Correspondants départementaux:
+PPC: Bérengère MONVOISIN
+77: Cyrille BOST
+78-95: Angélique EGLOFF
+91: Olivier MELART
+Assistance:
+assistance.geobs@ofb.gouv.fr</t>
   </si>
 </sst>
 </file>
@@ -1698,10 +1699,10 @@
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomRight" activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1855,7 +1856,7 @@
         <v>40</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>41</v>
@@ -1946,7 +1947,7 @@
         <v>66</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>67</v>
@@ -2553,7 +2554,7 @@
         <v>92</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -2775,7 +2776,7 @@
         <v>207</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>208</v>

</xml_diff>

<commit_message>
mise à jour des correspondants en SD
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3F71E1-4309-4199-83F1-49CD6E30D3F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC658539-3606-44EE-ABFA-8A71433F9231}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -793,9 +793,6 @@
     <t>Le ROE permet d’avoir une information spatialisée sur les obstacles à l’écoulement des cours d’eau d’origine humaine (caractéristiques, usages, gestion). Cette information peut être complétée dans la BDOE.</t>
   </si>
   <si>
-    <t>Collecter des informations objectives sur le nombre, la localisation et les caractéristiques des obstacles à l'écoulement sur les cours d'eau</t>
-  </si>
-  <si>
     <t>Elaboration d’un référentiel national et un socle commun d’information. Estimer la pression ouvrage sur les cours d'eau. 
 Suivi des politiques de restauration de la continuité écologique
 Calcul d’indicateurs de continuité écologique</t>
@@ -807,12 +804,6 @@
   <si>
     <t>Opportuniste ou plannifié
 A l'étiage pour la caractérisation des hauteurs de chute</t>
-  </si>
-  <si>
-    <t>Agence de l'eau
-DRIEAT
-Syndicats de rivière
-Fédérations de pêche</t>
   </si>
   <si>
     <t>Formé</t>
@@ -1030,30 +1021,6 @@
 Laurence CURTET
 Animation régionale:
 Samuel DEMBSKI</t>
-  </si>
-  <si>
-    <t>Animation nationale:
-Céline NOWAK
-Animation régionale:
-Samuel DEMBSKI
-Correspondants départementaux:
-PPC: Bérengère MONVOISIN
-77: Cyrille BOST
-78-95: Louis COQUELLE
-91: Alice PACAUD</t>
-  </si>
-  <si>
-    <t>Animation nationale:
-Nicolas JEAN
-Animation régionale:
-Samuel DEMBSKI
-Correspondants départementaux:
-PPC: Sylvain BERANGER
-77: Corinne REVEL
-78-95: Estelle DEBOST
-91: Philippe TURQUIN
-Courriel du réseau:
-reseau.loup-lynx@ofb.gouv.fr</t>
   </si>
   <si>
     <t>Animation nationale:
@@ -1064,48 +1031,6 @@
 Samuel DEMBSKI
 Courriel du réseau:
 reseau.becasse@ofb.gouv.fr</t>
-  </si>
-  <si>
-    <t>Animation nationale:
-Paul HUREL
-Suivi scientifique:
-Yoann BRESSAN
-Sandrine RUETTE
-Animation régionale:
-Cédric MONDY
-Correspondants départementaux:
-PPC: Sylvain BERANGER
-77: Anne-Gaëlle BLANC
-78-95: Amandine EVRARD
-91: Cyril KLEINPRINZ</t>
-  </si>
-  <si>
-    <t>Animation nationale:
-Paul HUREL
-Suivi scientifique:
-Yoann BRESSAN
-Référence technique:
-Laurence HENRY
-Animation régionale:
-Cédric MONDY
-Correspondants départementaux:
-PPC: Sylvain BERANGER
-77: Anne-Gaëlle BLANC
-78-95: Amandine EVRARD
-91: Cyril KLEINPRINZ</t>
-  </si>
-  <si>
-    <t>Animation nationale: 
-Karl KREUTZENBERGER
-Animation régionale:
-Cédric MONDY
-Correspondants départementaux:
-PPC: Bérengère MONVOISIN
-77: Cyrille BOST
-78-95: Angélique EGLOFF
-91: Olivier MELART
-Assistance:
-assistance.geobs@ofb.gouv.fr</t>
   </si>
   <si>
     <t>Animation nationale:
@@ -1127,6 +1052,84 @@
   </si>
   <si>
     <t>&lt; 5 minutes</t>
+  </si>
+  <si>
+    <t>Animation nationale:
+Paul HUREL
+Suivi scientifique:
+Maëlle TEYSSEIRE
+Yoann BRESSAN
+Animation régionale:
+Cédric MONDY
+Correspondants départementaux:
+PPC: 
+77: Anne-Gaëlle BLANC
+78-95: Amandine EVRARD
+91: Cyril KLEINPRINZ</t>
+  </si>
+  <si>
+    <t>Animation nationale:
+Paul HUREL
+Suivi scientifique:
+Yoann BRESSAN
+Référence technique:
+Laurence HENRY
+Maëlle TEYSSEIRE
+Animation régionale:
+Cédric MONDY
+Correspondants départementaux:
+PPC: 
+77: Anne-Gaëlle BLANC
+78-95: Amandine EVRARD
+91: Cyril KLEINPRINZ</t>
+  </si>
+  <si>
+    <t>Animation nationale:
+Nicolas JEAN
+Animation régionale:
+Samuel DEMBSKI
+Correspondants départementaux:
+PPC: 
+77: Corinne REVEL
+       Julien CURE
+78-95: Estelle DEBOST
+91: Philippe TURQUIN
+Courriel du réseau:
+reseau.loup-lynx@ofb.gouv.fr</t>
+  </si>
+  <si>
+    <t>Animation nationale:
+Céline NOWAK
+Animation régionale:
+Samuel DEMBSKI
+Correspondants départementaux:
+PPC: 
+77: Cyrille BOST
+78-95: Paul RIVAUD
+91: Alice PACAUD</t>
+  </si>
+  <si>
+    <t>Collecter et animer la collecte d'informations objectives sur le nombre, la localisation et les caractéristiques des obstacles à l'écoulement sur les cours d'eau</t>
+  </si>
+  <si>
+    <t>Agence de l'eau
+DRIEAT
+Syndicats de rivière
+Fédérations de pêche
+Collectivités</t>
+  </si>
+  <si>
+    <t>Animation nationale: 
+Karl KREUTZENBERGER
+Animation régionale:
+Cédric MONDY
+Correspondants départementaux:
+PPC: 
+77: Cyrille BOST
+78-95: Angélique EGLOFF
+91: Sébastien LANGUILLE
+Assistance:
+assistance.geobs@ofb.gouv.fr</t>
   </si>
 </sst>
 </file>
@@ -1696,10 +1699,10 @@
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O3" sqref="O3"/>
+      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1853,14 +1856,14 @@
         <v>40</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>41</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>42</v>
@@ -1944,14 +1947,14 @@
         <v>65</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>66</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>42</v>
@@ -2065,7 +2068,7 @@
         <v>92</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>93</v>
@@ -2153,7 +2156,7 @@
         <v>116</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>117</v>
@@ -2269,7 +2272,7 @@
         <v>140</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>141</v>
@@ -2551,7 +2554,7 @@
         <v>90</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -2659,14 +2662,14 @@
         <v>182</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>183</v>
       </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="P18" s="1" t="s">
         <v>184</v>
@@ -2756,10 +2759,10 @@
         <v>200</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>89</v>
@@ -2767,23 +2770,23 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="K20" s="1" t="s">
-        <v>204</v>
-      </c>
       <c r="L20" s="1" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>205</v>
+        <v>267</v>
       </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1" t="s">
         <v>94</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="Q20" s="1">
         <v>1</v>
@@ -2792,79 +2795,79 @@
         <v>163</v>
       </c>
       <c r="S20" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="U20" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="V20" s="1"/>
       <c r="W20" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="X20" s="1"/>
       <c r="Y20" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="AA20" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="Z20" s="1" t="s">
+      <c r="AB20" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="AA20" s="1" t="s">
+      <c r="AD20" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="AB20" s="1" t="s">
+      <c r="AE20" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="AD20" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="AE20" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:31" ht="330" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="D21" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="E21" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>42</v>
@@ -2879,72 +2882,72 @@
         <v>120</v>
       </c>
       <c r="T21" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="V21" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="U21" s="1" t="s">
+      <c r="W21" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="W21" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="X21" s="1" t="s">
         <v>74</v>
       </c>
       <c r="Y21" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="AA21" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="Z21" s="1" t="s">
+      <c r="AB21" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="AA21" s="1" t="s">
+      <c r="AD21" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="AB21" s="1" t="s">
+      <c r="AE21" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="AD21" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="AE21" s="1" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="22" spans="1:31" ht="255" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>89</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1" t="s">
@@ -2963,37 +2966,37 @@
         <v>120</v>
       </c>
       <c r="T22" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="U22" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="V22" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="U22" s="7" t="s">
+      <c r="W22" s="7" t="s">
         <v>249</v>
-      </c>
-      <c r="V22" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="W22" s="7" t="s">
-        <v>251</v>
       </c>
       <c r="X22" s="1"/>
       <c r="Y22" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="Z22" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="AA22" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="Z22" s="7" t="s">
+      <c r="AB22" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="AA22" s="1" t="s">
+      <c r="AC22" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="AB22" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="AC22" s="1" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -3023,7 +3026,7 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>

</xml_diff>

<commit_message>
premier jet de la fiche ongulés
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC658539-3606-44EE-ABFA-8A71433F9231}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC02DF29-E07E-45E3-A4D1-0DA7E794D09E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="279">
   <si>
     <t>suivi</t>
   </si>
@@ -1130,6 +1130,43 @@
 91: Sébastien LANGUILLE
 Assistance:
 assistance.geobs@ofb.gouv.fr</t>
+  </si>
+  <si>
+    <t>Réseau Ongulés sauvages</t>
+  </si>
+  <si>
+    <t>Le réseau a pour but de récolter les informations utiles pour suivre les 14 espèces d'ongulés sauvages présentes en France hexagonale</t>
+  </si>
+  <si>
+    <t>L’ensemble des données récoltées permet de mesurer de façon régulière des variables biologiques d’intérêt, telles que les aires de présence, les tendances d’évolution ou l’état de santé des populations d’ongulés sauvages en France métropolitaine. En parallèle, d’autres données connexes, telles les prélèvements cynégétiques ou les modalités de gestion des populations, sont régulièrement enregistrées.</t>
+  </si>
+  <si>
+    <t>Animation nationale: XXXX
+Animation régionale: Samuel DEMBSKI
+Correspondants départementaux:
+PPC:
+77:
+78-95:
+91
+Courriel du réseau: reseau.ongules-sauvages@ofb.gouv.fr</t>
+  </si>
+  <si>
+    <t>Fédérations de chasse</t>
+  </si>
+  <si>
+    <t>texte:Dataviz: Présence des ongulés sauvages en France;lien:https://professionnels.ofb.fr/fr/doc-dataviz/dataviz-presence-ongules-sauvages-en-France</t>
+  </si>
+  <si>
+    <t>texte:Fiches de synthèse des suivis;lien:https://professionnels.ofb.fr/fr/node/869</t>
+  </si>
+  <si>
+    <t>texte: Cartes de répartition;lien:https://carmen.carmencarto.fr/38/Ongules_sauvages.map#</t>
+  </si>
+  <si>
+    <t>texte:Lettre d'information;lien:https://professionnels.ofb.fr/fr/node/1281</t>
+  </si>
+  <si>
+    <t>texte: Page du réseau sur le portail technique;lien:https://professionnels.ofb.fr/node/1431</t>
   </si>
 </sst>
 </file>
@@ -1699,10 +1736,10 @@
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2005,22 +2042,36 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" ht="285" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>269</v>
+      </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
+      <c r="D4" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>271</v>
+      </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="K4" s="7"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="L4" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -2033,7 +2084,24 @@
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="7"/>
+      <c r="Z4" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="5" spans="1:32" ht="285" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@9f679cb034ef967e1d1a924d606f8fdd6adf62bd 🚀
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC658539-3606-44EE-ABFA-8A71433F9231}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC02DF29-E07E-45E3-A4D1-0DA7E794D09E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="279">
   <si>
     <t>suivi</t>
   </si>
@@ -1130,6 +1130,43 @@
 91: Sébastien LANGUILLE
 Assistance:
 assistance.geobs@ofb.gouv.fr</t>
+  </si>
+  <si>
+    <t>Réseau Ongulés sauvages</t>
+  </si>
+  <si>
+    <t>Le réseau a pour but de récolter les informations utiles pour suivre les 14 espèces d'ongulés sauvages présentes en France hexagonale</t>
+  </si>
+  <si>
+    <t>L’ensemble des données récoltées permet de mesurer de façon régulière des variables biologiques d’intérêt, telles que les aires de présence, les tendances d’évolution ou l’état de santé des populations d’ongulés sauvages en France métropolitaine. En parallèle, d’autres données connexes, telles les prélèvements cynégétiques ou les modalités de gestion des populations, sont régulièrement enregistrées.</t>
+  </si>
+  <si>
+    <t>Animation nationale: XXXX
+Animation régionale: Samuel DEMBSKI
+Correspondants départementaux:
+PPC:
+77:
+78-95:
+91
+Courriel du réseau: reseau.ongules-sauvages@ofb.gouv.fr</t>
+  </si>
+  <si>
+    <t>Fédérations de chasse</t>
+  </si>
+  <si>
+    <t>texte:Dataviz: Présence des ongulés sauvages en France;lien:https://professionnels.ofb.fr/fr/doc-dataviz/dataviz-presence-ongules-sauvages-en-France</t>
+  </si>
+  <si>
+    <t>texte:Fiches de synthèse des suivis;lien:https://professionnels.ofb.fr/fr/node/869</t>
+  </si>
+  <si>
+    <t>texte: Cartes de répartition;lien:https://carmen.carmencarto.fr/38/Ongules_sauvages.map#</t>
+  </si>
+  <si>
+    <t>texte:Lettre d'information;lien:https://professionnels.ofb.fr/fr/node/1281</t>
+  </si>
+  <si>
+    <t>texte: Page du réseau sur le portail technique;lien:https://professionnels.ofb.fr/node/1431</t>
   </si>
 </sst>
 </file>
@@ -1699,10 +1736,10 @@
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2005,22 +2042,36 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" ht="285" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>269</v>
+      </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
+      <c r="D4" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>271</v>
+      </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="K4" s="7"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="L4" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -2033,7 +2084,24 @@
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="7"/>
+      <c r="Z4" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="5" spans="1:32" ht="285" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">

</xml_diff>

<commit_message>
gestion des suivis intégrés dans les métadonnées
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC02DF29-E07E-45E3-A4D1-0DA7E794D09E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA1D979-2EC2-4ABD-BD2D-FF4C06FEE9B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="282">
   <si>
     <t>suivi</t>
   </si>
@@ -1168,12 +1168,21 @@
   <si>
     <t>texte: Page du réseau sur le portail technique;lien:https://professionnels.ofb.fr/node/1431</t>
   </si>
+  <si>
+    <t>publiable</t>
+  </si>
+  <si>
+    <t>oui</t>
+  </si>
+  <si>
+    <t>non</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1285,7 +1294,10 @@
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="33">
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1396,41 +1408,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B84CBB1B-C38F-41A7-A936-743876B1F305}" name="Tableau1" displayName="Tableau1" ref="A1:AF24" totalsRowShown="0">
-  <autoFilter ref="A1:AF24" xr:uid="{EF1B83D5-E66B-47E5-BA3E-4C83D3ECD89E}"/>
-  <tableColumns count="32">
-    <tableColumn id="1" xr3:uid="{5B39F531-B957-45E4-B8D7-A8EF89A02254}" name="suivi" dataDxfId="31"/>
-    <tableColumn id="25" xr3:uid="{782941AC-FB8B-4754-8CBF-02D0BAF2941E}" name="intitule" dataDxfId="30"/>
-    <tableColumn id="26" xr3:uid="{BCD01C6C-1CB9-4299-B7DF-54BB2D22D660}" name="logo" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{3CCA40E1-EC4D-4139-95C2-02E6782BD062}" name="description" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{D81FE419-C289-42FA-8BCC-DBC27CA6EAFB}" name="objectif" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{A2609BD0-68D5-4CE3-AA7C-307DBA79F26D}" name="utilisation" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{9EDCADB8-F525-494F-AC84-0692F3DACD06}" name="departements" dataDxfId="25"/>
-    <tableColumn id="22" xr3:uid="{658FF927-894F-4065-8AAB-82AFDE7177DD}" name="fichier_stations" dataDxfId="24"/>
-    <tableColumn id="33" xr3:uid="{F057330C-77BF-46B2-B91F-0EACE6C1913E}" name="forme_suivi" dataDxfId="23"/>
-    <tableColumn id="23" xr3:uid="{2D0ECED5-574B-49CC-984F-91CD0F19FFF6}" name="mois" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{84E8BB51-20B7-494C-9CE5-543FFD3DC8E0}" name="temporalite" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{78F5487C-EC17-4AFB-94FB-545CA9E7285C}" name="animation" dataDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{6B384EC0-FA0D-4A85-8C9A-1E120A15E2FC}" name="partenaires" dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{2F64F147-A984-4D54-83A0-29F317643399}" name="transversalite" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{29D5CB78-6BB9-49AD-A55A-A97CA9799332}" name="duree" dataDxfId="17"/>
-    <tableColumn id="12" xr3:uid="{869EED11-E2FC-46E0-ACF9-0DDC82CE3DC4}" name="expertise" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{C4310D48-97B0-4BC5-8D16-B16809824F9D}" name="nombre_agents" dataDxfId="15"/>
-    <tableColumn id="13" xr3:uid="{F4DBE069-BA7F-4080-94B2-8ABBF7538774}" name="role_national" dataDxfId="14"/>
-    <tableColumn id="14" xr3:uid="{258750F9-2A96-4283-887D-9CFA4D17F439}" name="role_regional" dataDxfId="13"/>
-    <tableColumn id="15" xr3:uid="{9871871F-54ED-487E-A03C-7A8C48D3CFC5}" name="role_departemental" dataDxfId="12"/>
-    <tableColumn id="24" xr3:uid="{FD209E5E-CC51-404C-B64E-C171238903FA}" name="droits_formations" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{199EAB2D-1AF2-4CDB-8DA8-9AFCF50D2515}" name="protocole" dataDxfId="10"/>
-    <tableColumn id="17" xr3:uid="{98D077C8-A3ED-4384-B70C-4A4280C26FE7}" name="materiel" dataDxfId="9"/>
-    <tableColumn id="18" xr3:uid="{5054FBBA-5094-4C33-92F7-7A30AFA38A22}" name="autres_releves" dataDxfId="8"/>
-    <tableColumn id="19" xr3:uid="{FD214916-9E0C-4234-853A-5FE7AF8CF557}" name="saisie_validation" dataDxfId="7"/>
-    <tableColumn id="20" xr3:uid="{214FE337-1EDA-4253-A78D-B9247E4FADAF}" name="diffusion" dataDxfId="6"/>
-    <tableColumn id="21" xr3:uid="{D5A66587-DDDF-4D32-897E-51F4D17676D7}" name="plus_recto1" dataDxfId="5"/>
-    <tableColumn id="29" xr3:uid="{68D7BF7D-E5CC-41EC-90C5-AF11729CC6D2}" name="plus_recto2" dataDxfId="4"/>
-    <tableColumn id="30" xr3:uid="{5A2652F8-BC92-4FC4-A98C-E430D61980AA}" name="plus_recto3" dataDxfId="3"/>
-    <tableColumn id="27" xr3:uid="{9293E153-542E-44B7-8608-6A7DF028B0AB}" name="plus_verso1" dataDxfId="2"/>
-    <tableColumn id="31" xr3:uid="{03BAB4B1-56CF-43A6-AFEC-CB2C3A01FBC2}" name="plus_verso2" dataDxfId="1"/>
-    <tableColumn id="32" xr3:uid="{A8A25170-2E24-4434-9B14-0CA372542DEF}" name="plus_verso3" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B84CBB1B-C38F-41A7-A936-743876B1F305}" name="Tableau1" displayName="Tableau1" ref="A1:AG24" totalsRowShown="0">
+  <autoFilter ref="A1:AG24" xr:uid="{EF1B83D5-E66B-47E5-BA3E-4C83D3ECD89E}"/>
+  <tableColumns count="33">
+    <tableColumn id="1" xr3:uid="{5B39F531-B957-45E4-B8D7-A8EF89A02254}" name="suivi" dataDxfId="32"/>
+    <tableColumn id="28" xr3:uid="{47A9009B-0B72-4938-A50E-776A9597A3EA}" name="publiable" dataDxfId="0"/>
+    <tableColumn id="25" xr3:uid="{782941AC-FB8B-4754-8CBF-02D0BAF2941E}" name="intitule" dataDxfId="31"/>
+    <tableColumn id="26" xr3:uid="{BCD01C6C-1CB9-4299-B7DF-54BB2D22D660}" name="logo" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{3CCA40E1-EC4D-4139-95C2-02E6782BD062}" name="description" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{D81FE419-C289-42FA-8BCC-DBC27CA6EAFB}" name="objectif" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{A2609BD0-68D5-4CE3-AA7C-307DBA79F26D}" name="utilisation" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{9EDCADB8-F525-494F-AC84-0692F3DACD06}" name="departements" dataDxfId="26"/>
+    <tableColumn id="22" xr3:uid="{658FF927-894F-4065-8AAB-82AFDE7177DD}" name="fichier_stations" dataDxfId="25"/>
+    <tableColumn id="33" xr3:uid="{F057330C-77BF-46B2-B91F-0EACE6C1913E}" name="forme_suivi" dataDxfId="24"/>
+    <tableColumn id="23" xr3:uid="{2D0ECED5-574B-49CC-984F-91CD0F19FFF6}" name="mois" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{84E8BB51-20B7-494C-9CE5-543FFD3DC8E0}" name="temporalite" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{78F5487C-EC17-4AFB-94FB-545CA9E7285C}" name="animation" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{6B384EC0-FA0D-4A85-8C9A-1E120A15E2FC}" name="partenaires" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{2F64F147-A984-4D54-83A0-29F317643399}" name="transversalite" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{29D5CB78-6BB9-49AD-A55A-A97CA9799332}" name="duree" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{869EED11-E2FC-46E0-ACF9-0DDC82CE3DC4}" name="expertise" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{C4310D48-97B0-4BC5-8D16-B16809824F9D}" name="nombre_agents" dataDxfId="16"/>
+    <tableColumn id="13" xr3:uid="{F4DBE069-BA7F-4080-94B2-8ABBF7538774}" name="role_national" dataDxfId="15"/>
+    <tableColumn id="14" xr3:uid="{258750F9-2A96-4283-887D-9CFA4D17F439}" name="role_regional" dataDxfId="14"/>
+    <tableColumn id="15" xr3:uid="{9871871F-54ED-487E-A03C-7A8C48D3CFC5}" name="role_departemental" dataDxfId="13"/>
+    <tableColumn id="24" xr3:uid="{FD209E5E-CC51-404C-B64E-C171238903FA}" name="droits_formations" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{199EAB2D-1AF2-4CDB-8DA8-9AFCF50D2515}" name="protocole" dataDxfId="11"/>
+    <tableColumn id="17" xr3:uid="{98D077C8-A3ED-4384-B70C-4A4280C26FE7}" name="materiel" dataDxfId="10"/>
+    <tableColumn id="18" xr3:uid="{5054FBBA-5094-4C33-92F7-7A30AFA38A22}" name="autres_releves" dataDxfId="9"/>
+    <tableColumn id="19" xr3:uid="{FD214916-9E0C-4234-853A-5FE7AF8CF557}" name="saisie_validation" dataDxfId="8"/>
+    <tableColumn id="20" xr3:uid="{214FE337-1EDA-4253-A78D-B9247E4FADAF}" name="diffusion" dataDxfId="7"/>
+    <tableColumn id="21" xr3:uid="{D5A66587-DDDF-4D32-897E-51F4D17676D7}" name="plus_recto1" dataDxfId="6"/>
+    <tableColumn id="29" xr3:uid="{68D7BF7D-E5CC-41EC-90C5-AF11729CC6D2}" name="plus_recto2" dataDxfId="5"/>
+    <tableColumn id="30" xr3:uid="{5A2652F8-BC92-4FC4-A98C-E430D61980AA}" name="plus_recto3" dataDxfId="4"/>
+    <tableColumn id="27" xr3:uid="{9293E153-542E-44B7-8608-6A7DF028B0AB}" name="plus_verso1" dataDxfId="3"/>
+    <tableColumn id="31" xr3:uid="{03BAB4B1-56CF-43A6-AFEC-CB2C3A01FBC2}" name="plus_verso2" dataDxfId="2"/>
+    <tableColumn id="32" xr3:uid="{A8A25170-2E24-4434-9B14-0CA372542DEF}" name="plus_verso3" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1733,559 +1746,579 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C57DFD-1CB4-4BB6-806B-B3A954B7C9AD}">
-  <dimension ref="A1:AF24"/>
+  <dimension ref="A1:AG24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="11.42578125" style="4"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
-    <col min="7" max="10" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="23.85546875" customWidth="1"/>
-    <col min="12" max="12" width="21.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1"/>
-    <col min="17" max="17" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="14.85546875" customWidth="1"/>
-    <col min="20" max="21" width="20.85546875" customWidth="1"/>
-    <col min="22" max="22" width="38.5703125" customWidth="1"/>
-    <col min="23" max="23" width="29" customWidth="1"/>
-    <col min="24" max="24" width="16" customWidth="1"/>
-    <col min="25" max="25" width="29.85546875" customWidth="1"/>
-    <col min="27" max="29" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="11.42578125" style="4"/>
+    <col min="5" max="5" width="37.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1"/>
+    <col min="8" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="23.85546875" customWidth="1"/>
+    <col min="13" max="13" width="21.28515625" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" customWidth="1"/>
+    <col min="18" max="18" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="14.85546875" customWidth="1"/>
+    <col min="21" max="22" width="20.85546875" customWidth="1"/>
+    <col min="23" max="23" width="38.5703125" customWidth="1"/>
+    <col min="24" max="24" width="29" customWidth="1"/>
+    <col min="25" max="25" width="16" customWidth="1"/>
+    <col min="26" max="26" width="29.85546875" customWidth="1"/>
+    <col min="28" max="30" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="285" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="285">
       <c r="A2" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="1"/>
+      <c r="J2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="1"/>
+      <c r="P2" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="R2" s="1">
         <v>1</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1" t="s">
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="315" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" ht="315">
       <c r="A3" s="5" t="s">
         <v>56</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="1"/>
+      <c r="P3" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="R3" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="W3" s="7" t="s">
+      <c r="X3" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AE3" s="1" t="s">
+      <c r="AF3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AG3" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:32" ht="285" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" ht="285">
       <c r="A4" s="5" t="s">
         <v>82</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2"/>
+      <c r="H4" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="1"/>
+      <c r="K4" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="7"/>
+      <c r="M4" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="7"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="7" t="s">
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="AB4" s="1" t="s">
+      <c r="AC4" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="AC4" s="1" t="s">
+      <c r="AD4" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AE4" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AF4" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="5" spans="1:32" ht="285" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" ht="285">
       <c r="A5" s="5" t="s">
         <v>83</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="D5" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="1"/>
+      <c r="P5" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="R5" s="1">
         <v>1</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="U5" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="U5" s="7" t="s">
+      <c r="V5" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="W5" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="X5" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="Y5" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Y5" s="7" t="s">
+      <c r="Z5" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="AA5" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AB5" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AE5" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="AE5" s="1" t="s">
+      <c r="AF5" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="AF5" s="1" t="s">
+      <c r="AG5" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:32" ht="255" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" ht="255">
       <c r="A6" s="5" t="s">
         <v>108</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>77</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="1"/>
+      <c r="J6" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1" t="s">
+      <c r="O6" s="1"/>
+      <c r="P6" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="R6" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="U6" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="V6" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="V6" s="7" t="s">
+      <c r="W6" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="W6" s="6" t="s">
+      <c r="X6" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="Y6" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="Y6" s="6" t="s">
+      <c r="Z6" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="Z6" s="6" t="s">
+      <c r="AA6" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AB6" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="AB6" s="1" t="s">
+      <c r="AC6" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="AD6" s="1" t="s">
+      <c r="AE6" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="AE6" s="1" t="s">
+      <c r="AF6" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33">
       <c r="A7" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="5"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -2308,86 +2341,92 @@
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
     </row>
-    <row r="8" spans="1:32" ht="285" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" ht="285">
       <c r="A8" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>77</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="1" t="s">
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="R8" s="1">
         <v>1</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="T8" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="U8" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1" t="s">
+      <c r="V8" s="1"/>
+      <c r="W8" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="W8" s="7" t="s">
+      <c r="X8" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
-      <c r="Z8" s="7" t="s">
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="AA8" s="1" t="s">
+      <c r="AB8" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="AD8" s="1" t="s">
+      <c r="AE8" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33">
       <c r="A9" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -2410,14 +2449,17 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33">
       <c r="A10" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="1"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -2440,14 +2482,17 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33">
       <c r="A11" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="1"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -2470,14 +2515,17 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33">
       <c r="A12" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="1"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -2500,14 +2548,17 @@
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33">
       <c r="A13" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -2530,14 +2581,17 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33">
       <c r="A14" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="1"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -2560,14 +2614,17 @@
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33">
       <c r="A15" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="1"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -2590,88 +2647,94 @@
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="1:32" ht="315" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" ht="315">
       <c r="A16" s="5" t="s">
         <v>156</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="5"/>
+      <c r="E16" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="F16" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="G16" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="1"/>
+      <c r="J16" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="M16" s="1"/>
       <c r="N16" s="1"/>
-      <c r="O16" s="1" t="s">
+      <c r="O16" s="1"/>
+      <c r="P16" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="Q16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="R16" s="1">
         <v>1</v>
       </c>
-      <c r="R16" s="1" t="s">
+      <c r="S16" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="S16" s="1" t="s">
+      <c r="T16" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="T16" s="1" t="s">
+      <c r="U16" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="U16" s="1" t="s">
+      <c r="V16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1" t="s">
+      <c r="W16" s="1"/>
+      <c r="X16" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1" t="s">
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="Z16" s="1" t="s">
+      <c r="AA16" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="AA16" s="1" t="s">
+      <c r="AB16" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="AD16" s="1" t="s">
+      <c r="AE16" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32">
       <c r="A17" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B17" s="5"/>
+      <c r="B17" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C17" s="5"/>
-      <c r="D17" s="1"/>
+      <c r="D17" s="5"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -2694,104 +2757,110 @@
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
     </row>
-    <row r="18" spans="1:31" ht="210" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32" ht="210">
       <c r="A18" s="5" t="s">
         <v>172</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="K18" s="7" t="s">
+      <c r="L18" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="M18" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1" t="s">
+      <c r="O18" s="1"/>
+      <c r="P18" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="Q18" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="Q18" s="1">
+      <c r="R18" s="1">
         <v>1</v>
       </c>
-      <c r="R18" s="1" t="s">
+      <c r="S18" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="S18" s="1" t="s">
+      <c r="T18" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="T18" s="1" t="s">
+      <c r="U18" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="U18" s="7" t="s">
+      <c r="V18" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="V18" s="1" t="s">
+      <c r="W18" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="W18" s="1" t="s">
+      <c r="X18" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="X18" s="1" t="s">
+      <c r="Y18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Y18" s="1" t="s">
+      <c r="Z18" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="Z18" s="7" t="s">
+      <c r="AA18" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="AA18" s="1" t="s">
+      <c r="AB18" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AB18" s="1" t="s">
+      <c r="AC18" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="AC18" s="1" t="s">
+      <c r="AD18" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="AD18" s="1" t="s">
+      <c r="AE18" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32">
       <c r="A19" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B19" s="5"/>
+      <c r="B19" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C19" s="5"/>
-      <c r="D19" s="1"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -2814,261 +2883,273 @@
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
     </row>
-    <row r="20" spans="1:31" ht="270" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" ht="270">
       <c r="A20" s="5" t="s">
         <v>198</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="5"/>
+      <c r="E20" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="1"/>
+      <c r="K20" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="N20" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1" t="s">
+      <c r="O20" s="1"/>
+      <c r="P20" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="Q20" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="Q20" s="1">
+      <c r="R20" s="1">
         <v>1</v>
       </c>
-      <c r="R20" s="1" t="s">
+      <c r="S20" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="S20" s="1" t="s">
+      <c r="T20" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="T20" s="1" t="s">
+      <c r="U20" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="U20" s="1" t="s">
+      <c r="V20" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="V20" s="1"/>
-      <c r="W20" s="7" t="s">
+      <c r="W20" s="1"/>
+      <c r="X20" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1" t="s">
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="Z20" s="1" t="s">
+      <c r="AA20" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="AA20" s="1" t="s">
+      <c r="AB20" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="AB20" s="1" t="s">
+      <c r="AC20" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="AD20" s="1" t="s">
+      <c r="AE20" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="AE20" s="1" t="s">
+      <c r="AF20" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="330" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32" ht="330">
       <c r="A21" s="5" t="s">
         <v>215</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1" t="s">
+      <c r="I21" s="1"/>
+      <c r="J21" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="N21" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1" t="s">
+      <c r="O21" s="1"/>
+      <c r="P21" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="P21" s="1" t="s">
+      <c r="Q21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q21" s="1">
+      <c r="R21" s="1">
         <v>5</v>
       </c>
-      <c r="R21" s="1" t="s">
+      <c r="S21" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="S21" s="1" t="s">
+      <c r="T21" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="T21" s="1" t="s">
+      <c r="U21" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="U21" s="1" t="s">
+      <c r="V21" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="V21" s="1" t="s">
+      <c r="W21" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="W21" s="1" t="s">
+      <c r="X21" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="X21" s="1" t="s">
+      <c r="Y21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Y21" s="7" t="s">
+      <c r="Z21" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="Z21" s="1" t="s">
+      <c r="AA21" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="AA21" s="1" t="s">
+      <c r="AB21" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="AB21" s="1" t="s">
+      <c r="AC21" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="AD21" s="1" t="s">
+      <c r="AE21" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="AE21" s="1" t="s">
+      <c r="AF21" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="255" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" ht="255">
       <c r="A22" s="5" t="s">
         <v>237</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="5"/>
+      <c r="E22" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1" t="s">
+      <c r="I22" s="1"/>
+      <c r="J22" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1" t="s">
+      <c r="L22" s="1"/>
+      <c r="M22" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="N22" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1" t="s">
+      <c r="O22" s="1"/>
+      <c r="P22" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="Q22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q22" s="1">
+      <c r="R22" s="1">
         <v>1</v>
       </c>
-      <c r="R22" s="1" t="s">
+      <c r="S22" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="S22" s="1" t="s">
+      <c r="T22" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="T22" s="1" t="s">
+      <c r="U22" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="U22" s="7" t="s">
+      <c r="V22" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="V22" s="1" t="s">
+      <c r="W22" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="W22" s="7" t="s">
+      <c r="X22" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="7" t="s">
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="Z22" s="7" t="s">
+      <c r="AA22" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="AA22" s="1" t="s">
+      <c r="AB22" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="AB22" s="1" t="s">
+      <c r="AC22" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="AC22" s="1" t="s">
+      <c r="AD22" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32">
       <c r="A23" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="B23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="1"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -3091,14 +3172,17 @@
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32">
       <c r="A24" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="B24" s="5"/>
+      <c r="B24" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="1"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -3121,10 +3205,11 @@
       <c r="X24" s="1"/>
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" xr:uid="{27C333FC-2187-470A-9EAE-03AF18F8C27F}"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{27C333FC-2187-470A-9EAE-03AF18F8C27F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ OFB-IdF/src_idf@f414681594728107609ec090e78e0ccabc608098 🚀
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedric.mondy\Documents\_DRIDF\05_CONNAISSANCE\08_VALORISATION\src_idf\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC02DF29-E07E-45E3-A4D1-0DA7E794D09E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA1D979-2EC2-4ABD-BD2D-FF4C06FEE9B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7650" xr2:uid="{222ABCEC-F2C3-4E13-B88E-28B2CED8E82C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="282">
   <si>
     <t>suivi</t>
   </si>
@@ -1168,12 +1168,21 @@
   <si>
     <t>texte: Page du réseau sur le portail technique;lien:https://professionnels.ofb.fr/node/1431</t>
   </si>
+  <si>
+    <t>publiable</t>
+  </si>
+  <si>
+    <t>oui</t>
+  </si>
+  <si>
+    <t>non</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1285,7 +1294,10 @@
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="33">
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1396,41 +1408,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B84CBB1B-C38F-41A7-A936-743876B1F305}" name="Tableau1" displayName="Tableau1" ref="A1:AF24" totalsRowShown="0">
-  <autoFilter ref="A1:AF24" xr:uid="{EF1B83D5-E66B-47E5-BA3E-4C83D3ECD89E}"/>
-  <tableColumns count="32">
-    <tableColumn id="1" xr3:uid="{5B39F531-B957-45E4-B8D7-A8EF89A02254}" name="suivi" dataDxfId="31"/>
-    <tableColumn id="25" xr3:uid="{782941AC-FB8B-4754-8CBF-02D0BAF2941E}" name="intitule" dataDxfId="30"/>
-    <tableColumn id="26" xr3:uid="{BCD01C6C-1CB9-4299-B7DF-54BB2D22D660}" name="logo" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{3CCA40E1-EC4D-4139-95C2-02E6782BD062}" name="description" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{D81FE419-C289-42FA-8BCC-DBC27CA6EAFB}" name="objectif" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{A2609BD0-68D5-4CE3-AA7C-307DBA79F26D}" name="utilisation" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{9EDCADB8-F525-494F-AC84-0692F3DACD06}" name="departements" dataDxfId="25"/>
-    <tableColumn id="22" xr3:uid="{658FF927-894F-4065-8AAB-82AFDE7177DD}" name="fichier_stations" dataDxfId="24"/>
-    <tableColumn id="33" xr3:uid="{F057330C-77BF-46B2-B91F-0EACE6C1913E}" name="forme_suivi" dataDxfId="23"/>
-    <tableColumn id="23" xr3:uid="{2D0ECED5-574B-49CC-984F-91CD0F19FFF6}" name="mois" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{84E8BB51-20B7-494C-9CE5-543FFD3DC8E0}" name="temporalite" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{78F5487C-EC17-4AFB-94FB-545CA9E7285C}" name="animation" dataDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{6B384EC0-FA0D-4A85-8C9A-1E120A15E2FC}" name="partenaires" dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{2F64F147-A984-4D54-83A0-29F317643399}" name="transversalite" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{29D5CB78-6BB9-49AD-A55A-A97CA9799332}" name="duree" dataDxfId="17"/>
-    <tableColumn id="12" xr3:uid="{869EED11-E2FC-46E0-ACF9-0DDC82CE3DC4}" name="expertise" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{C4310D48-97B0-4BC5-8D16-B16809824F9D}" name="nombre_agents" dataDxfId="15"/>
-    <tableColumn id="13" xr3:uid="{F4DBE069-BA7F-4080-94B2-8ABBF7538774}" name="role_national" dataDxfId="14"/>
-    <tableColumn id="14" xr3:uid="{258750F9-2A96-4283-887D-9CFA4D17F439}" name="role_regional" dataDxfId="13"/>
-    <tableColumn id="15" xr3:uid="{9871871F-54ED-487E-A03C-7A8C48D3CFC5}" name="role_departemental" dataDxfId="12"/>
-    <tableColumn id="24" xr3:uid="{FD209E5E-CC51-404C-B64E-C171238903FA}" name="droits_formations" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{199EAB2D-1AF2-4CDB-8DA8-9AFCF50D2515}" name="protocole" dataDxfId="10"/>
-    <tableColumn id="17" xr3:uid="{98D077C8-A3ED-4384-B70C-4A4280C26FE7}" name="materiel" dataDxfId="9"/>
-    <tableColumn id="18" xr3:uid="{5054FBBA-5094-4C33-92F7-7A30AFA38A22}" name="autres_releves" dataDxfId="8"/>
-    <tableColumn id="19" xr3:uid="{FD214916-9E0C-4234-853A-5FE7AF8CF557}" name="saisie_validation" dataDxfId="7"/>
-    <tableColumn id="20" xr3:uid="{214FE337-1EDA-4253-A78D-B9247E4FADAF}" name="diffusion" dataDxfId="6"/>
-    <tableColumn id="21" xr3:uid="{D5A66587-DDDF-4D32-897E-51F4D17676D7}" name="plus_recto1" dataDxfId="5"/>
-    <tableColumn id="29" xr3:uid="{68D7BF7D-E5CC-41EC-90C5-AF11729CC6D2}" name="plus_recto2" dataDxfId="4"/>
-    <tableColumn id="30" xr3:uid="{5A2652F8-BC92-4FC4-A98C-E430D61980AA}" name="plus_recto3" dataDxfId="3"/>
-    <tableColumn id="27" xr3:uid="{9293E153-542E-44B7-8608-6A7DF028B0AB}" name="plus_verso1" dataDxfId="2"/>
-    <tableColumn id="31" xr3:uid="{03BAB4B1-56CF-43A6-AFEC-CB2C3A01FBC2}" name="plus_verso2" dataDxfId="1"/>
-    <tableColumn id="32" xr3:uid="{A8A25170-2E24-4434-9B14-0CA372542DEF}" name="plus_verso3" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B84CBB1B-C38F-41A7-A936-743876B1F305}" name="Tableau1" displayName="Tableau1" ref="A1:AG24" totalsRowShown="0">
+  <autoFilter ref="A1:AG24" xr:uid="{EF1B83D5-E66B-47E5-BA3E-4C83D3ECD89E}"/>
+  <tableColumns count="33">
+    <tableColumn id="1" xr3:uid="{5B39F531-B957-45E4-B8D7-A8EF89A02254}" name="suivi" dataDxfId="32"/>
+    <tableColumn id="28" xr3:uid="{47A9009B-0B72-4938-A50E-776A9597A3EA}" name="publiable" dataDxfId="0"/>
+    <tableColumn id="25" xr3:uid="{782941AC-FB8B-4754-8CBF-02D0BAF2941E}" name="intitule" dataDxfId="31"/>
+    <tableColumn id="26" xr3:uid="{BCD01C6C-1CB9-4299-B7DF-54BB2D22D660}" name="logo" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{3CCA40E1-EC4D-4139-95C2-02E6782BD062}" name="description" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{D81FE419-C289-42FA-8BCC-DBC27CA6EAFB}" name="objectif" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{A2609BD0-68D5-4CE3-AA7C-307DBA79F26D}" name="utilisation" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{9EDCADB8-F525-494F-AC84-0692F3DACD06}" name="departements" dataDxfId="26"/>
+    <tableColumn id="22" xr3:uid="{658FF927-894F-4065-8AAB-82AFDE7177DD}" name="fichier_stations" dataDxfId="25"/>
+    <tableColumn id="33" xr3:uid="{F057330C-77BF-46B2-B91F-0EACE6C1913E}" name="forme_suivi" dataDxfId="24"/>
+    <tableColumn id="23" xr3:uid="{2D0ECED5-574B-49CC-984F-91CD0F19FFF6}" name="mois" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{84E8BB51-20B7-494C-9CE5-543FFD3DC8E0}" name="temporalite" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{78F5487C-EC17-4AFB-94FB-545CA9E7285C}" name="animation" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{6B384EC0-FA0D-4A85-8C9A-1E120A15E2FC}" name="partenaires" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{2F64F147-A984-4D54-83A0-29F317643399}" name="transversalite" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{29D5CB78-6BB9-49AD-A55A-A97CA9799332}" name="duree" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{869EED11-E2FC-46E0-ACF9-0DDC82CE3DC4}" name="expertise" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{C4310D48-97B0-4BC5-8D16-B16809824F9D}" name="nombre_agents" dataDxfId="16"/>
+    <tableColumn id="13" xr3:uid="{F4DBE069-BA7F-4080-94B2-8ABBF7538774}" name="role_national" dataDxfId="15"/>
+    <tableColumn id="14" xr3:uid="{258750F9-2A96-4283-887D-9CFA4D17F439}" name="role_regional" dataDxfId="14"/>
+    <tableColumn id="15" xr3:uid="{9871871F-54ED-487E-A03C-7A8C48D3CFC5}" name="role_departemental" dataDxfId="13"/>
+    <tableColumn id="24" xr3:uid="{FD209E5E-CC51-404C-B64E-C171238903FA}" name="droits_formations" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{199EAB2D-1AF2-4CDB-8DA8-9AFCF50D2515}" name="protocole" dataDxfId="11"/>
+    <tableColumn id="17" xr3:uid="{98D077C8-A3ED-4384-B70C-4A4280C26FE7}" name="materiel" dataDxfId="10"/>
+    <tableColumn id="18" xr3:uid="{5054FBBA-5094-4C33-92F7-7A30AFA38A22}" name="autres_releves" dataDxfId="9"/>
+    <tableColumn id="19" xr3:uid="{FD214916-9E0C-4234-853A-5FE7AF8CF557}" name="saisie_validation" dataDxfId="8"/>
+    <tableColumn id="20" xr3:uid="{214FE337-1EDA-4253-A78D-B9247E4FADAF}" name="diffusion" dataDxfId="7"/>
+    <tableColumn id="21" xr3:uid="{D5A66587-DDDF-4D32-897E-51F4D17676D7}" name="plus_recto1" dataDxfId="6"/>
+    <tableColumn id="29" xr3:uid="{68D7BF7D-E5CC-41EC-90C5-AF11729CC6D2}" name="plus_recto2" dataDxfId="5"/>
+    <tableColumn id="30" xr3:uid="{5A2652F8-BC92-4FC4-A98C-E430D61980AA}" name="plus_recto3" dataDxfId="4"/>
+    <tableColumn id="27" xr3:uid="{9293E153-542E-44B7-8608-6A7DF028B0AB}" name="plus_verso1" dataDxfId="3"/>
+    <tableColumn id="31" xr3:uid="{03BAB4B1-56CF-43A6-AFEC-CB2C3A01FBC2}" name="plus_verso2" dataDxfId="2"/>
+    <tableColumn id="32" xr3:uid="{A8A25170-2E24-4434-9B14-0CA372542DEF}" name="plus_verso3" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1733,559 +1746,579 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C57DFD-1CB4-4BB6-806B-B3A954B7C9AD}">
-  <dimension ref="A1:AF24"/>
+  <dimension ref="A1:AG24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="11.42578125" style="4"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
-    <col min="7" max="10" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="23.85546875" customWidth="1"/>
-    <col min="12" max="12" width="21.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1"/>
-    <col min="17" max="17" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="14.85546875" customWidth="1"/>
-    <col min="20" max="21" width="20.85546875" customWidth="1"/>
-    <col min="22" max="22" width="38.5703125" customWidth="1"/>
-    <col min="23" max="23" width="29" customWidth="1"/>
-    <col min="24" max="24" width="16" customWidth="1"/>
-    <col min="25" max="25" width="29.85546875" customWidth="1"/>
-    <col min="27" max="29" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="11.42578125" style="4"/>
+    <col min="5" max="5" width="37.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1"/>
+    <col min="8" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="23.85546875" customWidth="1"/>
+    <col min="13" max="13" width="21.28515625" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" customWidth="1"/>
+    <col min="18" max="18" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="14.85546875" customWidth="1"/>
+    <col min="21" max="22" width="20.85546875" customWidth="1"/>
+    <col min="23" max="23" width="38.5703125" customWidth="1"/>
+    <col min="24" max="24" width="29" customWidth="1"/>
+    <col min="25" max="25" width="16" customWidth="1"/>
+    <col min="26" max="26" width="29.85546875" customWidth="1"/>
+    <col min="28" max="30" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="285" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="285">
       <c r="A2" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="1"/>
+      <c r="J2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="1"/>
+      <c r="P2" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="R2" s="1">
         <v>1</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1" t="s">
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="315" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" ht="315">
       <c r="A3" s="5" t="s">
         <v>56</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="1"/>
+      <c r="P3" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="R3" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="W3" s="7" t="s">
+      <c r="X3" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AE3" s="1" t="s">
+      <c r="AF3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AG3" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:32" ht="285" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" ht="285">
       <c r="A4" s="5" t="s">
         <v>82</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2"/>
+      <c r="H4" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="1"/>
+      <c r="K4" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="7"/>
+      <c r="M4" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="7"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="7" t="s">
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="AB4" s="1" t="s">
+      <c r="AC4" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="AC4" s="1" t="s">
+      <c r="AD4" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AE4" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AF4" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="5" spans="1:32" ht="285" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" ht="285">
       <c r="A5" s="5" t="s">
         <v>83</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="D5" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="1"/>
+      <c r="P5" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="R5" s="1">
         <v>1</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="U5" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="U5" s="7" t="s">
+      <c r="V5" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="W5" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="X5" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="Y5" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Y5" s="7" t="s">
+      <c r="Z5" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="AA5" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AB5" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AE5" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="AE5" s="1" t="s">
+      <c r="AF5" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="AF5" s="1" t="s">
+      <c r="AG5" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:32" ht="255" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" ht="255">
       <c r="A6" s="5" t="s">
         <v>108</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>77</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="1"/>
+      <c r="J6" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1" t="s">
+      <c r="O6" s="1"/>
+      <c r="P6" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="R6" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="U6" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="V6" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="V6" s="7" t="s">
+      <c r="W6" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="W6" s="6" t="s">
+      <c r="X6" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="Y6" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="Y6" s="6" t="s">
+      <c r="Z6" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="Z6" s="6" t="s">
+      <c r="AA6" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AB6" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="AB6" s="1" t="s">
+      <c r="AC6" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="AD6" s="1" t="s">
+      <c r="AE6" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="AE6" s="1" t="s">
+      <c r="AF6" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33">
       <c r="A7" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="5"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -2308,86 +2341,92 @@
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
     </row>
-    <row r="8" spans="1:32" ht="285" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" ht="285">
       <c r="A8" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>77</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="1" t="s">
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="R8" s="1">
         <v>1</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="T8" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="U8" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1" t="s">
+      <c r="V8" s="1"/>
+      <c r="W8" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="W8" s="7" t="s">
+      <c r="X8" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
-      <c r="Z8" s="7" t="s">
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="AA8" s="1" t="s">
+      <c r="AB8" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="AD8" s="1" t="s">
+      <c r="AE8" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33">
       <c r="A9" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -2410,14 +2449,17 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33">
       <c r="A10" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="1"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -2440,14 +2482,17 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33">
       <c r="A11" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="1"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -2470,14 +2515,17 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33">
       <c r="A12" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="1"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -2500,14 +2548,17 @@
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33">
       <c r="A13" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -2530,14 +2581,17 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33">
       <c r="A14" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="1"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -2560,14 +2614,17 @@
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33">
       <c r="A15" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="1"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -2590,88 +2647,94 @@
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="1:32" ht="315" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" ht="315">
       <c r="A16" s="5" t="s">
         <v>156</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="5"/>
+      <c r="E16" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="F16" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="G16" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="1"/>
+      <c r="J16" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="M16" s="1"/>
       <c r="N16" s="1"/>
-      <c r="O16" s="1" t="s">
+      <c r="O16" s="1"/>
+      <c r="P16" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="Q16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="R16" s="1">
         <v>1</v>
       </c>
-      <c r="R16" s="1" t="s">
+      <c r="S16" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="S16" s="1" t="s">
+      <c r="T16" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="T16" s="1" t="s">
+      <c r="U16" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="U16" s="1" t="s">
+      <c r="V16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1" t="s">
+      <c r="W16" s="1"/>
+      <c r="X16" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1" t="s">
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="Z16" s="1" t="s">
+      <c r="AA16" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="AA16" s="1" t="s">
+      <c r="AB16" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="AD16" s="1" t="s">
+      <c r="AE16" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32">
       <c r="A17" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B17" s="5"/>
+      <c r="B17" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C17" s="5"/>
-      <c r="D17" s="1"/>
+      <c r="D17" s="5"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -2694,104 +2757,110 @@
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
     </row>
-    <row r="18" spans="1:31" ht="210" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32" ht="210">
       <c r="A18" s="5" t="s">
         <v>172</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="K18" s="7" t="s">
+      <c r="L18" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="M18" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1" t="s">
+      <c r="O18" s="1"/>
+      <c r="P18" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="Q18" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="Q18" s="1">
+      <c r="R18" s="1">
         <v>1</v>
       </c>
-      <c r="R18" s="1" t="s">
+      <c r="S18" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="S18" s="1" t="s">
+      <c r="T18" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="T18" s="1" t="s">
+      <c r="U18" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="U18" s="7" t="s">
+      <c r="V18" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="V18" s="1" t="s">
+      <c r="W18" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="W18" s="1" t="s">
+      <c r="X18" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="X18" s="1" t="s">
+      <c r="Y18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Y18" s="1" t="s">
+      <c r="Z18" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="Z18" s="7" t="s">
+      <c r="AA18" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="AA18" s="1" t="s">
+      <c r="AB18" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AB18" s="1" t="s">
+      <c r="AC18" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="AC18" s="1" t="s">
+      <c r="AD18" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="AD18" s="1" t="s">
+      <c r="AE18" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32">
       <c r="A19" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B19" s="5"/>
+      <c r="B19" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C19" s="5"/>
-      <c r="D19" s="1"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -2814,261 +2883,273 @@
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
     </row>
-    <row r="20" spans="1:31" ht="270" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" ht="270">
       <c r="A20" s="5" t="s">
         <v>198</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="5"/>
+      <c r="E20" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="1"/>
+      <c r="K20" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="N20" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1" t="s">
+      <c r="O20" s="1"/>
+      <c r="P20" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="Q20" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="Q20" s="1">
+      <c r="R20" s="1">
         <v>1</v>
       </c>
-      <c r="R20" s="1" t="s">
+      <c r="S20" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="S20" s="1" t="s">
+      <c r="T20" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="T20" s="1" t="s">
+      <c r="U20" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="U20" s="1" t="s">
+      <c r="V20" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="V20" s="1"/>
-      <c r="W20" s="7" t="s">
+      <c r="W20" s="1"/>
+      <c r="X20" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1" t="s">
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="Z20" s="1" t="s">
+      <c r="AA20" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="AA20" s="1" t="s">
+      <c r="AB20" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="AB20" s="1" t="s">
+      <c r="AC20" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="AD20" s="1" t="s">
+      <c r="AE20" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="AE20" s="1" t="s">
+      <c r="AF20" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="330" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32" ht="330">
       <c r="A21" s="5" t="s">
         <v>215</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1" t="s">
+      <c r="I21" s="1"/>
+      <c r="J21" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="N21" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1" t="s">
+      <c r="O21" s="1"/>
+      <c r="P21" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="P21" s="1" t="s">
+      <c r="Q21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q21" s="1">
+      <c r="R21" s="1">
         <v>5</v>
       </c>
-      <c r="R21" s="1" t="s">
+      <c r="S21" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="S21" s="1" t="s">
+      <c r="T21" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="T21" s="1" t="s">
+      <c r="U21" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="U21" s="1" t="s">
+      <c r="V21" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="V21" s="1" t="s">
+      <c r="W21" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="W21" s="1" t="s">
+      <c r="X21" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="X21" s="1" t="s">
+      <c r="Y21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Y21" s="7" t="s">
+      <c r="Z21" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="Z21" s="1" t="s">
+      <c r="AA21" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="AA21" s="1" t="s">
+      <c r="AB21" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="AB21" s="1" t="s">
+      <c r="AC21" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="AD21" s="1" t="s">
+      <c r="AE21" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="AE21" s="1" t="s">
+      <c r="AF21" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="255" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" ht="255">
       <c r="A22" s="5" t="s">
         <v>237</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="5"/>
+      <c r="E22" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1" t="s">
+      <c r="I22" s="1"/>
+      <c r="J22" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1" t="s">
+      <c r="L22" s="1"/>
+      <c r="M22" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="N22" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1" t="s">
+      <c r="O22" s="1"/>
+      <c r="P22" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="Q22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q22" s="1">
+      <c r="R22" s="1">
         <v>1</v>
       </c>
-      <c r="R22" s="1" t="s">
+      <c r="S22" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="S22" s="1" t="s">
+      <c r="T22" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="T22" s="1" t="s">
+      <c r="U22" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="U22" s="7" t="s">
+      <c r="V22" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="V22" s="1" t="s">
+      <c r="W22" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="W22" s="7" t="s">
+      <c r="X22" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="7" t="s">
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="Z22" s="7" t="s">
+      <c r="AA22" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="AA22" s="1" t="s">
+      <c r="AB22" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="AB22" s="1" t="s">
+      <c r="AC22" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="AC22" s="1" t="s">
+      <c r="AD22" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32">
       <c r="A23" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="B23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="1"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -3091,14 +3172,17 @@
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32">
       <c r="A24" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="B24" s="5"/>
+      <c r="B24" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="1"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -3121,10 +3205,11 @@
       <c r="X24" s="1"/>
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" xr:uid="{27C333FC-2187-470A-9EAE-03AF18F8C27F}"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{27C333FC-2187-470A-9EAE-03AF18F8C27F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>